<commit_message>
enny06 2019/12/11 13.03 modified datetime
</commit_message>
<xml_diff>
--- a/assets/templates/unlock/template_users_log.xlsx
+++ b/assets/templates/unlock/template_users_log.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\greebel\assets\templates\unlock\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7A9278-EB35-41AA-8386-F4490E69D93E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20055" windowHeight="7935"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -33,12 +46,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,7 +141,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -177,13 +190,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -230,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,9 +289,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,6 +341,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -471,20 +534,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O533"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="11" width="9.140625" style="21"/>
     <col min="14" max="14" width="9.140625" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25">
+    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -501,7 +564,7 @@
       <c r="N1" s="14"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -516,13 +579,13 @@
       <c r="H3" s="12"/>
       <c r="I3" s="19"/>
       <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="K3" s="22"/>
       <c r="L3" s="10"/>
       <c r="M3" s="1"/>
       <c r="N3" s="14"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
@@ -535,13 +598,13 @@
       <c r="H4" s="11"/>
       <c r="I4" s="19"/>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="10"/>
       <c r="M4" s="1"/>
       <c r="N4" s="14"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -560,7 +623,7 @@
       <c r="N5" s="14"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -577,7 +640,7 @@
       <c r="N6" s="14"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -594,7 +657,7 @@
       <c r="N7" s="18"/>
       <c r="O7" s="5"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
@@ -611,7 +674,7 @@
       <c r="N8" s="13"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="5"/>
@@ -628,7 +691,7 @@
       <c r="N9" s="13"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="5"/>
@@ -645,7 +708,7 @@
       <c r="N10" s="13"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
@@ -662,7 +725,7 @@
       <c r="N11" s="13"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
@@ -679,7 +742,7 @@
       <c r="N12" s="13"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -696,7 +759,7 @@
       <c r="N13" s="13"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="5"/>
@@ -713,7 +776,7 @@
       <c r="N14" s="13"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
@@ -730,7 +793,7 @@
       <c r="N15" s="13"/>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
@@ -747,7 +810,7 @@
       <c r="N16" s="13"/>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="5"/>
@@ -763,7 +826,7 @@
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5"/>
@@ -779,7 +842,7 @@
       <c r="M18" s="13"/>
       <c r="N18" s="13"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
@@ -795,7 +858,7 @@
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
@@ -811,7 +874,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="13"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="5"/>
@@ -827,7 +890,7 @@
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="5"/>
@@ -843,7 +906,7 @@
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
@@ -859,7 +922,7 @@
       <c r="M23" s="13"/>
       <c r="N23" s="13"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
@@ -875,7 +938,7 @@
       <c r="M24" s="13"/>
       <c r="N24" s="13"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="5"/>
@@ -891,7 +954,7 @@
       <c r="M25" s="13"/>
       <c r="N25" s="13"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5"/>
@@ -907,7 +970,7 @@
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="5"/>
@@ -923,7 +986,7 @@
       <c r="M27" s="13"/>
       <c r="N27" s="13"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="5"/>
@@ -939,7 +1002,7 @@
       <c r="M28" s="13"/>
       <c r="N28" s="13"/>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="5"/>
@@ -955,7 +1018,7 @@
       <c r="M29" s="13"/>
       <c r="N29" s="13"/>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="5"/>
@@ -971,7 +1034,7 @@
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="5"/>
@@ -987,7 +1050,7 @@
       <c r="M31" s="13"/>
       <c r="N31" s="13"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5"/>
@@ -1003,7 +1066,7 @@
       <c r="M32" s="13"/>
       <c r="N32" s="13"/>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="5"/>
@@ -1019,7 +1082,7 @@
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="5"/>
@@ -1035,7 +1098,7 @@
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -1051,7 +1114,7 @@
       <c r="M35" s="13"/>
       <c r="N35" s="13"/>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="5"/>
@@ -1067,7 +1130,7 @@
       <c r="M36" s="13"/>
       <c r="N36" s="13"/>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="5"/>
@@ -1083,7 +1146,7 @@
       <c r="M37" s="13"/>
       <c r="N37" s="13"/>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="5"/>
@@ -1099,7 +1162,7 @@
       <c r="M38" s="13"/>
       <c r="N38" s="13"/>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="5"/>
@@ -1115,7 +1178,7 @@
       <c r="M39" s="13"/>
       <c r="N39" s="13"/>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="5"/>
@@ -1131,7 +1194,7 @@
       <c r="M40" s="13"/>
       <c r="N40" s="13"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="5"/>
@@ -1147,7 +1210,7 @@
       <c r="M41" s="13"/>
       <c r="N41" s="13"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="5"/>
@@ -1163,7 +1226,7 @@
       <c r="M42" s="13"/>
       <c r="N42" s="13"/>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="5"/>
@@ -1179,7 +1242,7 @@
       <c r="M43" s="13"/>
       <c r="N43" s="13"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5"/>
@@ -1195,7 +1258,7 @@
       <c r="M44" s="13"/>
       <c r="N44" s="13"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="5"/>
@@ -1211,7 +1274,7 @@
       <c r="M45" s="13"/>
       <c r="N45" s="13"/>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="1"/>
@@ -1227,7 +1290,7 @@
       <c r="M46" s="13"/>
       <c r="N46" s="13"/>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="1"/>
@@ -1243,7 +1306,7 @@
       <c r="M47" s="13"/>
       <c r="N47" s="13"/>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="1"/>
@@ -1259,7 +1322,7 @@
       <c r="M48" s="13"/>
       <c r="N48" s="13"/>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="1"/>
@@ -1275,7 +1338,7 @@
       <c r="M49" s="13"/>
       <c r="N49" s="13"/>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="1"/>
@@ -1291,7 +1354,7 @@
       <c r="M50" s="13"/>
       <c r="N50" s="13"/>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="1"/>
@@ -1307,7 +1370,7 @@
       <c r="M51" s="13"/>
       <c r="N51" s="13"/>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="1"/>
@@ -1323,7 +1386,7 @@
       <c r="M52" s="13"/>
       <c r="N52" s="13"/>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="1"/>
@@ -1339,7 +1402,7 @@
       <c r="M53" s="13"/>
       <c r="N53" s="13"/>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="1"/>
@@ -1355,7 +1418,7 @@
       <c r="M54" s="13"/>
       <c r="N54" s="13"/>
     </row>
-    <row r="55" spans="1:14">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="1"/>
@@ -1371,7 +1434,7 @@
       <c r="M55" s="13"/>
       <c r="N55" s="13"/>
     </row>
-    <row r="56" spans="1:14">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="1"/>
@@ -1387,7 +1450,7 @@
       <c r="M56" s="13"/>
       <c r="N56" s="13"/>
     </row>
-    <row r="57" spans="1:14">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="1"/>
@@ -1403,7 +1466,7 @@
       <c r="M57" s="13"/>
       <c r="N57" s="13"/>
     </row>
-    <row r="58" spans="1:14">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="1"/>
@@ -1419,7 +1482,7 @@
       <c r="M58" s="13"/>
       <c r="N58" s="13"/>
     </row>
-    <row r="59" spans="1:14">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="1"/>
@@ -1435,7 +1498,7 @@
       <c r="M59" s="13"/>
       <c r="N59" s="13"/>
     </row>
-    <row r="60" spans="1:14">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="1"/>
@@ -1451,7 +1514,7 @@
       <c r="M60" s="13"/>
       <c r="N60" s="13"/>
     </row>
-    <row r="61" spans="1:14">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="1"/>
@@ -1467,7 +1530,7 @@
       <c r="M61" s="13"/>
       <c r="N61" s="13"/>
     </row>
-    <row r="62" spans="1:14">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="1"/>
@@ -1483,7 +1546,7 @@
       <c r="M62" s="13"/>
       <c r="N62" s="13"/>
     </row>
-    <row r="63" spans="1:14">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="1"/>
@@ -1499,7 +1562,7 @@
       <c r="M63" s="13"/>
       <c r="N63" s="13"/>
     </row>
-    <row r="64" spans="1:14">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="1"/>
@@ -1515,7 +1578,7 @@
       <c r="M64" s="13"/>
       <c r="N64" s="13"/>
     </row>
-    <row r="65" spans="1:14">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="1"/>
@@ -1531,7 +1594,7 @@
       <c r="M65" s="13"/>
       <c r="N65" s="13"/>
     </row>
-    <row r="66" spans="1:14">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="1"/>
@@ -1547,7 +1610,7 @@
       <c r="M66" s="13"/>
       <c r="N66" s="13"/>
     </row>
-    <row r="67" spans="1:14">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="1"/>
@@ -1563,7 +1626,7 @@
       <c r="M67" s="13"/>
       <c r="N67" s="13"/>
     </row>
-    <row r="68" spans="1:14">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="1"/>
@@ -1579,7 +1642,7 @@
       <c r="M68" s="13"/>
       <c r="N68" s="13"/>
     </row>
-    <row r="69" spans="1:14">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="1"/>
@@ -1595,7 +1658,7 @@
       <c r="M69" s="13"/>
       <c r="N69" s="13"/>
     </row>
-    <row r="70" spans="1:14">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="1"/>
@@ -1611,7 +1674,7 @@
       <c r="M70" s="13"/>
       <c r="N70" s="13"/>
     </row>
-    <row r="71" spans="1:14">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="1"/>
@@ -1627,7 +1690,7 @@
       <c r="M71" s="13"/>
       <c r="N71" s="13"/>
     </row>
-    <row r="72" spans="1:14">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="1"/>
@@ -1643,7 +1706,7 @@
       <c r="M72" s="13"/>
       <c r="N72" s="13"/>
     </row>
-    <row r="73" spans="1:14">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="1"/>
@@ -1659,7 +1722,7 @@
       <c r="M73" s="13"/>
       <c r="N73" s="13"/>
     </row>
-    <row r="74" spans="1:14">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="1"/>
@@ -1675,7 +1738,7 @@
       <c r="M74" s="13"/>
       <c r="N74" s="13"/>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="1"/>
@@ -1691,7 +1754,7 @@
       <c r="M75" s="13"/>
       <c r="N75" s="13"/>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="1"/>
@@ -1707,7 +1770,7 @@
       <c r="M76" s="13"/>
       <c r="N76" s="13"/>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="1"/>
@@ -1723,7 +1786,7 @@
       <c r="M77" s="13"/>
       <c r="N77" s="13"/>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="1"/>
@@ -1739,7 +1802,7 @@
       <c r="M78" s="13"/>
       <c r="N78" s="13"/>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="1"/>
@@ -1755,7 +1818,7 @@
       <c r="M79" s="13"/>
       <c r="N79" s="13"/>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="1"/>
@@ -1771,7 +1834,7 @@
       <c r="M80" s="13"/>
       <c r="N80" s="13"/>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="1"/>
@@ -1787,7 +1850,7 @@
       <c r="M81" s="13"/>
       <c r="N81" s="13"/>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="1"/>
@@ -1803,7 +1866,7 @@
       <c r="M82" s="13"/>
       <c r="N82" s="13"/>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="1"/>
@@ -1819,7 +1882,7 @@
       <c r="M83" s="13"/>
       <c r="N83" s="13"/>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="1"/>
@@ -1835,7 +1898,7 @@
       <c r="M84" s="13"/>
       <c r="N84" s="13"/>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="1"/>
@@ -1851,7 +1914,7 @@
       <c r="M85" s="13"/>
       <c r="N85" s="13"/>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="1"/>
@@ -1867,7 +1930,7 @@
       <c r="M86" s="13"/>
       <c r="N86" s="13"/>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="1"/>
@@ -1883,7 +1946,7 @@
       <c r="M87" s="13"/>
       <c r="N87" s="13"/>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="1"/>
@@ -1899,7 +1962,7 @@
       <c r="M88" s="13"/>
       <c r="N88" s="13"/>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="1"/>
@@ -1915,7 +1978,7 @@
       <c r="M89" s="13"/>
       <c r="N89" s="13"/>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="1"/>
@@ -1931,7 +1994,7 @@
       <c r="M90" s="13"/>
       <c r="N90" s="13"/>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="1"/>
@@ -1947,7 +2010,7 @@
       <c r="M91" s="13"/>
       <c r="N91" s="13"/>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="1"/>
@@ -1963,7 +2026,7 @@
       <c r="M92" s="13"/>
       <c r="N92" s="13"/>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="1"/>
@@ -1979,7 +2042,7 @@
       <c r="M93" s="13"/>
       <c r="N93" s="13"/>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="1"/>
@@ -1995,7 +2058,7 @@
       <c r="M94" s="13"/>
       <c r="N94" s="13"/>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="1"/>
@@ -2011,7 +2074,7 @@
       <c r="M95" s="13"/>
       <c r="N95" s="13"/>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="1"/>
@@ -2027,7 +2090,7 @@
       <c r="M96" s="13"/>
       <c r="N96" s="13"/>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="1"/>
@@ -2043,7 +2106,7 @@
       <c r="M97" s="13"/>
       <c r="N97" s="13"/>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="1"/>
@@ -2059,7 +2122,7 @@
       <c r="M98" s="13"/>
       <c r="N98" s="13"/>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="1"/>
@@ -2075,7 +2138,7 @@
       <c r="M99" s="13"/>
       <c r="N99" s="13"/>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="3"/>
       <c r="B100" s="3"/>
       <c r="C100" s="1"/>
@@ -2091,7 +2154,7 @@
       <c r="M100" s="13"/>
       <c r="N100" s="13"/>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="3"/>
       <c r="B101" s="3"/>
       <c r="C101" s="1"/>
@@ -2107,7 +2170,7 @@
       <c r="M101" s="13"/>
       <c r="N101" s="13"/>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
       <c r="C102" s="1"/>
@@ -2123,7 +2186,7 @@
       <c r="M102" s="13"/>
       <c r="N102" s="13"/>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="3"/>
       <c r="B103" s="3"/>
       <c r="C103" s="1"/>
@@ -2139,7 +2202,7 @@
       <c r="M103" s="13"/>
       <c r="N103" s="13"/>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="3"/>
       <c r="B104" s="3"/>
       <c r="C104" s="1"/>
@@ -2155,7 +2218,7 @@
       <c r="M104" s="13"/>
       <c r="N104" s="13"/>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="3"/>
       <c r="B105" s="3"/>
       <c r="C105" s="1"/>
@@ -2171,7 +2234,7 @@
       <c r="M105" s="13"/>
       <c r="N105" s="13"/>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="3"/>
       <c r="B106" s="3"/>
       <c r="C106" s="1"/>
@@ -2187,7 +2250,7 @@
       <c r="M106" s="13"/>
       <c r="N106" s="13"/>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="1"/>
@@ -2203,7 +2266,7 @@
       <c r="M107" s="13"/>
       <c r="N107" s="13"/>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="1"/>
       <c r="B108" s="3"/>
       <c r="C108" s="1"/>
@@ -2219,7 +2282,7 @@
       <c r="M108" s="13"/>
       <c r="N108" s="13"/>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="1"/>
       <c r="B109" s="3"/>
       <c r="C109" s="1"/>
@@ -2235,7 +2298,7 @@
       <c r="M109" s="13"/>
       <c r="N109" s="13"/>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="1"/>
       <c r="B110" s="3"/>
       <c r="C110" s="1"/>
@@ -2251,7 +2314,7 @@
       <c r="M110" s="13"/>
       <c r="N110" s="13"/>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="1"/>
       <c r="B111" s="3"/>
       <c r="C111" s="1"/>
@@ -2267,7 +2330,7 @@
       <c r="M111" s="1"/>
       <c r="N111" s="13"/>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="1"/>
       <c r="B112" s="3"/>
       <c r="C112" s="1"/>
@@ -2283,7 +2346,7 @@
       <c r="M112" s="1"/>
       <c r="N112" s="13"/>
     </row>
-    <row r="113" spans="2:14">
+    <row r="113" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B113" s="3"/>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
@@ -2298,7 +2361,7 @@
       <c r="M113" s="1"/>
       <c r="N113" s="13"/>
     </row>
-    <row r="114" spans="2:14">
+    <row r="114" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B114" s="3"/>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
@@ -2313,7 +2376,7 @@
       <c r="M114" s="1"/>
       <c r="N114" s="13"/>
     </row>
-    <row r="115" spans="2:14">
+    <row r="115" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B115" s="3"/>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
@@ -2328,7 +2391,7 @@
       <c r="M115" s="1"/>
       <c r="N115" s="13"/>
     </row>
-    <row r="116" spans="2:14">
+    <row r="116" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B116" s="3"/>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
@@ -2343,7 +2406,7 @@
       <c r="M116" s="1"/>
       <c r="N116" s="13"/>
     </row>
-    <row r="117" spans="2:14">
+    <row r="117" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B117" s="3"/>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -2358,7 +2421,7 @@
       <c r="M117" s="1"/>
       <c r="N117" s="13"/>
     </row>
-    <row r="118" spans="2:14">
+    <row r="118" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B118" s="3"/>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -2373,7 +2436,7 @@
       <c r="M118" s="1"/>
       <c r="N118" s="13"/>
     </row>
-    <row r="119" spans="2:14">
+    <row r="119" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B119" s="3"/>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -2388,7 +2451,7 @@
       <c r="M119" s="1"/>
       <c r="N119" s="13"/>
     </row>
-    <row r="120" spans="2:14">
+    <row r="120" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B120" s="3"/>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -2403,7 +2466,7 @@
       <c r="M120" s="1"/>
       <c r="N120" s="13"/>
     </row>
-    <row r="121" spans="2:14">
+    <row r="121" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B121" s="3"/>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -2418,7 +2481,7 @@
       <c r="M121" s="1"/>
       <c r="N121" s="13"/>
     </row>
-    <row r="122" spans="2:14">
+    <row r="122" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B122" s="3"/>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -2433,7 +2496,7 @@
       <c r="M122" s="1"/>
       <c r="N122" s="13"/>
     </row>
-    <row r="123" spans="2:14">
+    <row r="123" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B123" s="3"/>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -2448,7 +2511,7 @@
       <c r="M123" s="1"/>
       <c r="N123" s="13"/>
     </row>
-    <row r="124" spans="2:14">
+    <row r="124" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B124" s="3"/>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -2463,7 +2526,7 @@
       <c r="M124" s="1"/>
       <c r="N124" s="13"/>
     </row>
-    <row r="125" spans="2:14">
+    <row r="125" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B125" s="3"/>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -2478,7 +2541,7 @@
       <c r="M125" s="1"/>
       <c r="N125" s="13"/>
     </row>
-    <row r="126" spans="2:14">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B126" s="3"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -2493,7 +2556,7 @@
       <c r="M126" s="1"/>
       <c r="N126" s="13"/>
     </row>
-    <row r="127" spans="2:14">
+    <row r="127" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B127" s="3"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -2508,7 +2571,7 @@
       <c r="M127" s="1"/>
       <c r="N127" s="13"/>
     </row>
-    <row r="128" spans="2:14">
+    <row r="128" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B128" s="3"/>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -2523,7 +2586,7 @@
       <c r="M128" s="1"/>
       <c r="N128" s="13"/>
     </row>
-    <row r="129" spans="2:14">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B129" s="3"/>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -2538,7 +2601,7 @@
       <c r="M129" s="1"/>
       <c r="N129" s="13"/>
     </row>
-    <row r="130" spans="2:14">
+    <row r="130" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B130" s="3"/>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -2553,7 +2616,7 @@
       <c r="M130" s="1"/>
       <c r="N130" s="13"/>
     </row>
-    <row r="131" spans="2:14">
+    <row r="131" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B131" s="3"/>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -2568,7 +2631,7 @@
       <c r="M131" s="1"/>
       <c r="N131" s="13"/>
     </row>
-    <row r="132" spans="2:14">
+    <row r="132" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B132" s="3"/>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -2583,7 +2646,7 @@
       <c r="M132" s="1"/>
       <c r="N132" s="13"/>
     </row>
-    <row r="133" spans="2:14">
+    <row r="133" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B133" s="3"/>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -2598,7 +2661,7 @@
       <c r="M133" s="1"/>
       <c r="N133" s="13"/>
     </row>
-    <row r="134" spans="2:14">
+    <row r="134" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B134" s="3"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -2613,7 +2676,7 @@
       <c r="M134" s="1"/>
       <c r="N134" s="13"/>
     </row>
-    <row r="135" spans="2:14">
+    <row r="135" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B135" s="3"/>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -2628,7 +2691,7 @@
       <c r="M135" s="1"/>
       <c r="N135" s="13"/>
     </row>
-    <row r="136" spans="2:14">
+    <row r="136" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B136" s="3"/>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -2643,7 +2706,7 @@
       <c r="M136" s="1"/>
       <c r="N136" s="13"/>
     </row>
-    <row r="137" spans="2:14">
+    <row r="137" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B137" s="3"/>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -2658,7 +2721,7 @@
       <c r="M137" s="1"/>
       <c r="N137" s="13"/>
     </row>
-    <row r="138" spans="2:14">
+    <row r="138" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B138" s="3"/>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -2673,7 +2736,7 @@
       <c r="M138" s="1"/>
       <c r="N138" s="13"/>
     </row>
-    <row r="139" spans="2:14">
+    <row r="139" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B139" s="3"/>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -2688,7 +2751,7 @@
       <c r="M139" s="1"/>
       <c r="N139" s="13"/>
     </row>
-    <row r="140" spans="2:14">
+    <row r="140" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B140" s="3"/>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -2703,7 +2766,7 @@
       <c r="M140" s="1"/>
       <c r="N140" s="13"/>
     </row>
-    <row r="141" spans="2:14">
+    <row r="141" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B141" s="3"/>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -2718,7 +2781,7 @@
       <c r="M141" s="1"/>
       <c r="N141" s="13"/>
     </row>
-    <row r="142" spans="2:14">
+    <row r="142" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B142" s="3"/>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -2733,7 +2796,7 @@
       <c r="M142" s="1"/>
       <c r="N142" s="13"/>
     </row>
-    <row r="143" spans="2:14">
+    <row r="143" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B143" s="3"/>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -2748,7 +2811,7 @@
       <c r="M143" s="1"/>
       <c r="N143" s="13"/>
     </row>
-    <row r="144" spans="2:14">
+    <row r="144" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B144" s="3"/>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -2763,7 +2826,7 @@
       <c r="M144" s="1"/>
       <c r="N144" s="13"/>
     </row>
-    <row r="145" spans="2:14">
+    <row r="145" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B145" s="3"/>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -2778,7 +2841,7 @@
       <c r="M145" s="1"/>
       <c r="N145" s="13"/>
     </row>
-    <row r="146" spans="2:14">
+    <row r="146" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B146" s="3"/>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -2793,7 +2856,7 @@
       <c r="M146" s="1"/>
       <c r="N146" s="13"/>
     </row>
-    <row r="147" spans="2:14">
+    <row r="147" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B147" s="3"/>
       <c r="C147" s="1"/>
       <c r="D147" s="1"/>
@@ -2808,7 +2871,7 @@
       <c r="M147" s="1"/>
       <c r="N147" s="13"/>
     </row>
-    <row r="148" spans="2:14">
+    <row r="148" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B148" s="3"/>
       <c r="C148" s="1"/>
       <c r="D148" s="1"/>
@@ -2823,7 +2886,7 @@
       <c r="M148" s="1"/>
       <c r="N148" s="13"/>
     </row>
-    <row r="149" spans="2:14">
+    <row r="149" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B149" s="3"/>
       <c r="C149" s="1"/>
       <c r="D149" s="1"/>
@@ -2838,7 +2901,7 @@
       <c r="M149" s="1"/>
       <c r="N149" s="13"/>
     </row>
-    <row r="150" spans="2:14">
+    <row r="150" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B150" s="3"/>
       <c r="C150" s="1"/>
       <c r="D150" s="1"/>
@@ -2853,7 +2916,7 @@
       <c r="M150" s="1"/>
       <c r="N150" s="13"/>
     </row>
-    <row r="151" spans="2:14">
+    <row r="151" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B151" s="3"/>
       <c r="C151" s="1"/>
       <c r="D151" s="1"/>
@@ -2868,7 +2931,7 @@
       <c r="M151" s="1"/>
       <c r="N151" s="13"/>
     </row>
-    <row r="152" spans="2:14">
+    <row r="152" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B152" s="3"/>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -2883,7 +2946,7 @@
       <c r="M152" s="1"/>
       <c r="N152" s="13"/>
     </row>
-    <row r="153" spans="2:14">
+    <row r="153" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B153" s="3"/>
       <c r="C153" s="1"/>
       <c r="D153" s="1"/>
@@ -2898,7 +2961,7 @@
       <c r="M153" s="1"/>
       <c r="N153" s="13"/>
     </row>
-    <row r="154" spans="2:14">
+    <row r="154" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B154" s="3"/>
       <c r="C154" s="1"/>
       <c r="D154" s="1"/>
@@ -2913,7 +2976,7 @@
       <c r="M154" s="1"/>
       <c r="N154" s="13"/>
     </row>
-    <row r="155" spans="2:14">
+    <row r="155" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B155" s="3"/>
       <c r="C155" s="1"/>
       <c r="D155" s="1"/>
@@ -2928,7 +2991,7 @@
       <c r="M155" s="1"/>
       <c r="N155" s="13"/>
     </row>
-    <row r="156" spans="2:14">
+    <row r="156" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B156" s="3"/>
       <c r="C156" s="1"/>
       <c r="D156" s="1"/>
@@ -2943,7 +3006,7 @@
       <c r="M156" s="1"/>
       <c r="N156" s="13"/>
     </row>
-    <row r="157" spans="2:14">
+    <row r="157" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B157" s="3"/>
       <c r="C157" s="1"/>
       <c r="D157" s="1"/>
@@ -2958,7 +3021,7 @@
       <c r="M157" s="1"/>
       <c r="N157" s="13"/>
     </row>
-    <row r="158" spans="2:14">
+    <row r="158" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B158" s="3"/>
       <c r="C158" s="1"/>
       <c r="D158" s="1"/>
@@ -2973,7 +3036,7 @@
       <c r="M158" s="1"/>
       <c r="N158" s="13"/>
     </row>
-    <row r="159" spans="2:14">
+    <row r="159" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B159" s="3"/>
       <c r="C159" s="1"/>
       <c r="D159" s="1"/>
@@ -2988,7 +3051,7 @@
       <c r="M159" s="1"/>
       <c r="N159" s="13"/>
     </row>
-    <row r="160" spans="2:14">
+    <row r="160" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B160" s="3"/>
       <c r="C160" s="1"/>
       <c r="D160" s="1"/>
@@ -3003,7 +3066,7 @@
       <c r="M160" s="1"/>
       <c r="N160" s="13"/>
     </row>
-    <row r="161" spans="2:14">
+    <row r="161" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B161" s="3"/>
       <c r="C161" s="1"/>
       <c r="D161" s="1"/>
@@ -3018,7 +3081,7 @@
       <c r="M161" s="1"/>
       <c r="N161" s="13"/>
     </row>
-    <row r="162" spans="2:14">
+    <row r="162" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B162" s="3"/>
       <c r="C162" s="1"/>
       <c r="D162" s="1"/>
@@ -3033,7 +3096,7 @@
       <c r="M162" s="1"/>
       <c r="N162" s="13"/>
     </row>
-    <row r="163" spans="2:14">
+    <row r="163" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B163" s="3"/>
       <c r="C163" s="1"/>
       <c r="D163" s="1"/>
@@ -3048,7 +3111,7 @@
       <c r="M163" s="1"/>
       <c r="N163" s="13"/>
     </row>
-    <row r="164" spans="2:14">
+    <row r="164" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B164" s="3"/>
       <c r="C164" s="1"/>
       <c r="D164" s="1"/>
@@ -3063,7 +3126,7 @@
       <c r="M164" s="1"/>
       <c r="N164" s="13"/>
     </row>
-    <row r="165" spans="2:14">
+    <row r="165" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B165" s="3"/>
       <c r="C165" s="1"/>
       <c r="D165" s="1"/>
@@ -3078,7 +3141,7 @@
       <c r="M165" s="1"/>
       <c r="N165" s="13"/>
     </row>
-    <row r="166" spans="2:14">
+    <row r="166" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B166" s="3"/>
       <c r="C166" s="1"/>
       <c r="D166" s="1"/>
@@ -3093,7 +3156,7 @@
       <c r="M166" s="1"/>
       <c r="N166" s="13"/>
     </row>
-    <row r="167" spans="2:14">
+    <row r="167" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B167" s="3"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -3108,7 +3171,7 @@
       <c r="M167" s="1"/>
       <c r="N167" s="13"/>
     </row>
-    <row r="168" spans="2:14">
+    <row r="168" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B168" s="3"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -3123,7 +3186,7 @@
       <c r="M168" s="1"/>
       <c r="N168" s="13"/>
     </row>
-    <row r="169" spans="2:14">
+    <row r="169" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B169" s="3"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -3138,7 +3201,7 @@
       <c r="M169" s="1"/>
       <c r="N169" s="13"/>
     </row>
-    <row r="170" spans="2:14">
+    <row r="170" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B170" s="3"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
@@ -3153,7 +3216,7 @@
       <c r="M170" s="1"/>
       <c r="N170" s="13"/>
     </row>
-    <row r="171" spans="2:14">
+    <row r="171" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B171" s="3"/>
       <c r="C171" s="1"/>
       <c r="D171" s="1"/>
@@ -3168,7 +3231,7 @@
       <c r="M171" s="1"/>
       <c r="N171" s="13"/>
     </row>
-    <row r="172" spans="2:14">
+    <row r="172" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B172" s="3"/>
       <c r="C172" s="1"/>
       <c r="D172" s="1"/>
@@ -3183,7 +3246,7 @@
       <c r="M172" s="1"/>
       <c r="N172" s="13"/>
     </row>
-    <row r="173" spans="2:14">
+    <row r="173" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B173" s="3"/>
       <c r="C173" s="1"/>
       <c r="D173" s="1"/>
@@ -3198,7 +3261,7 @@
       <c r="M173" s="1"/>
       <c r="N173" s="13"/>
     </row>
-    <row r="174" spans="2:14">
+    <row r="174" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B174" s="3"/>
       <c r="C174" s="1"/>
       <c r="D174" s="1"/>
@@ -3213,7 +3276,7 @@
       <c r="M174" s="1"/>
       <c r="N174" s="13"/>
     </row>
-    <row r="175" spans="2:14">
+    <row r="175" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B175" s="3"/>
       <c r="C175" s="1"/>
       <c r="D175" s="1"/>
@@ -3228,7 +3291,7 @@
       <c r="M175" s="1"/>
       <c r="N175" s="13"/>
     </row>
-    <row r="176" spans="2:14">
+    <row r="176" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B176" s="3"/>
       <c r="C176" s="1"/>
       <c r="D176" s="1"/>
@@ -3243,7 +3306,7 @@
       <c r="M176" s="1"/>
       <c r="N176" s="13"/>
     </row>
-    <row r="177" spans="2:14">
+    <row r="177" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B177" s="3"/>
       <c r="C177" s="1"/>
       <c r="D177" s="1"/>
@@ -3258,7 +3321,7 @@
       <c r="M177" s="1"/>
       <c r="N177" s="13"/>
     </row>
-    <row r="178" spans="2:14">
+    <row r="178" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B178" s="3"/>
       <c r="C178" s="1"/>
       <c r="D178" s="1"/>
@@ -3273,7 +3336,7 @@
       <c r="M178" s="1"/>
       <c r="N178" s="13"/>
     </row>
-    <row r="179" spans="2:14">
+    <row r="179" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B179" s="3"/>
       <c r="C179" s="1"/>
       <c r="D179" s="1"/>
@@ -3288,7 +3351,7 @@
       <c r="M179" s="1"/>
       <c r="N179" s="13"/>
     </row>
-    <row r="180" spans="2:14">
+    <row r="180" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B180" s="3"/>
       <c r="C180" s="1"/>
       <c r="D180" s="1"/>
@@ -3303,7 +3366,7 @@
       <c r="M180" s="1"/>
       <c r="N180" s="13"/>
     </row>
-    <row r="181" spans="2:14">
+    <row r="181" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B181" s="3"/>
       <c r="C181" s="1"/>
       <c r="D181" s="1"/>
@@ -3318,7 +3381,7 @@
       <c r="M181" s="1"/>
       <c r="N181" s="13"/>
     </row>
-    <row r="182" spans="2:14">
+    <row r="182" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B182" s="3"/>
       <c r="C182" s="1"/>
       <c r="D182" s="1"/>
@@ -3333,7 +3396,7 @@
       <c r="M182" s="1"/>
       <c r="N182" s="13"/>
     </row>
-    <row r="183" spans="2:14">
+    <row r="183" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B183" s="3"/>
       <c r="C183" s="1"/>
       <c r="D183" s="1"/>
@@ -3348,7 +3411,7 @@
       <c r="M183" s="1"/>
       <c r="N183" s="13"/>
     </row>
-    <row r="184" spans="2:14">
+    <row r="184" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B184" s="3"/>
       <c r="C184" s="1"/>
       <c r="D184" s="1"/>
@@ -3363,7 +3426,7 @@
       <c r="M184" s="1"/>
       <c r="N184" s="13"/>
     </row>
-    <row r="185" spans="2:14">
+    <row r="185" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B185" s="3"/>
       <c r="C185" s="1"/>
       <c r="D185" s="1"/>
@@ -3378,7 +3441,7 @@
       <c r="M185" s="1"/>
       <c r="N185" s="13"/>
     </row>
-    <row r="186" spans="2:14">
+    <row r="186" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B186" s="3"/>
       <c r="C186" s="1"/>
       <c r="D186" s="1"/>
@@ -3393,7 +3456,7 @@
       <c r="M186" s="1"/>
       <c r="N186" s="13"/>
     </row>
-    <row r="187" spans="2:14">
+    <row r="187" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B187" s="3"/>
       <c r="C187" s="1"/>
       <c r="D187" s="1"/>
@@ -3408,7 +3471,7 @@
       <c r="M187" s="1"/>
       <c r="N187" s="13"/>
     </row>
-    <row r="188" spans="2:14">
+    <row r="188" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B188" s="3"/>
       <c r="C188" s="1"/>
       <c r="D188" s="1"/>
@@ -3423,7 +3486,7 @@
       <c r="M188" s="1"/>
       <c r="N188" s="13"/>
     </row>
-    <row r="189" spans="2:14">
+    <row r="189" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B189" s="3"/>
       <c r="C189" s="1"/>
       <c r="D189" s="1"/>
@@ -3438,7 +3501,7 @@
       <c r="M189" s="1"/>
       <c r="N189" s="13"/>
     </row>
-    <row r="190" spans="2:14">
+    <row r="190" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B190" s="3"/>
       <c r="C190" s="1"/>
       <c r="D190" s="1"/>
@@ -3453,7 +3516,7 @@
       <c r="M190" s="1"/>
       <c r="N190" s="13"/>
     </row>
-    <row r="191" spans="2:14">
+    <row r="191" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B191" s="3"/>
       <c r="C191" s="1"/>
       <c r="D191" s="1"/>
@@ -3468,7 +3531,7 @@
       <c r="M191" s="1"/>
       <c r="N191" s="13"/>
     </row>
-    <row r="192" spans="2:14">
+    <row r="192" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B192" s="3"/>
       <c r="C192" s="1"/>
       <c r="D192" s="1"/>
@@ -3483,7 +3546,7 @@
       <c r="M192" s="1"/>
       <c r="N192" s="13"/>
     </row>
-    <row r="193" spans="2:14">
+    <row r="193" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B193" s="3"/>
       <c r="C193" s="1"/>
       <c r="D193" s="1"/>
@@ -3498,7 +3561,7 @@
       <c r="M193" s="1"/>
       <c r="N193" s="13"/>
     </row>
-    <row r="194" spans="2:14">
+    <row r="194" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B194" s="3"/>
       <c r="C194" s="1"/>
       <c r="D194" s="1"/>
@@ -3513,7 +3576,7 @@
       <c r="M194" s="1"/>
       <c r="N194" s="13"/>
     </row>
-    <row r="195" spans="2:14">
+    <row r="195" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B195" s="3"/>
       <c r="C195" s="1"/>
       <c r="D195" s="1"/>
@@ -3528,7 +3591,7 @@
       <c r="M195" s="1"/>
       <c r="N195" s="13"/>
     </row>
-    <row r="196" spans="2:14">
+    <row r="196" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B196" s="3"/>
       <c r="C196" s="1"/>
       <c r="D196" s="1"/>
@@ -3543,7 +3606,7 @@
       <c r="M196" s="1"/>
       <c r="N196" s="13"/>
     </row>
-    <row r="197" spans="2:14">
+    <row r="197" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B197" s="3"/>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -3558,7 +3621,7 @@
       <c r="M197" s="1"/>
       <c r="N197" s="13"/>
     </row>
-    <row r="198" spans="2:14">
+    <row r="198" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B198" s="3"/>
       <c r="C198" s="1"/>
       <c r="D198" s="1"/>
@@ -3573,7 +3636,7 @@
       <c r="M198" s="1"/>
       <c r="N198" s="13"/>
     </row>
-    <row r="199" spans="2:14">
+    <row r="199" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B199" s="3"/>
       <c r="C199" s="1"/>
       <c r="D199" s="1"/>
@@ -3588,7 +3651,7 @@
       <c r="M199" s="1"/>
       <c r="N199" s="13"/>
     </row>
-    <row r="200" spans="2:14">
+    <row r="200" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B200" s="3"/>
       <c r="C200" s="1"/>
       <c r="D200" s="1"/>
@@ -3603,7 +3666,7 @@
       <c r="M200" s="1"/>
       <c r="N200" s="13"/>
     </row>
-    <row r="201" spans="2:14">
+    <row r="201" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B201" s="3"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -3618,7 +3681,7 @@
       <c r="M201" s="1"/>
       <c r="N201" s="13"/>
     </row>
-    <row r="202" spans="2:14">
+    <row r="202" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B202" s="3"/>
       <c r="C202" s="1"/>
       <c r="D202" s="1"/>
@@ -3633,7 +3696,7 @@
       <c r="M202" s="1"/>
       <c r="N202" s="13"/>
     </row>
-    <row r="203" spans="2:14">
+    <row r="203" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B203" s="3"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -3648,7 +3711,7 @@
       <c r="M203" s="1"/>
       <c r="N203" s="13"/>
     </row>
-    <row r="204" spans="2:14">
+    <row r="204" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B204" s="3"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -3663,7 +3726,7 @@
       <c r="M204" s="1"/>
       <c r="N204" s="13"/>
     </row>
-    <row r="205" spans="2:14">
+    <row r="205" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B205" s="3"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -3678,7 +3741,7 @@
       <c r="M205" s="1"/>
       <c r="N205" s="13"/>
     </row>
-    <row r="206" spans="2:14">
+    <row r="206" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B206" s="3"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -3693,7 +3756,7 @@
       <c r="M206" s="1"/>
       <c r="N206" s="13"/>
     </row>
-    <row r="207" spans="2:14">
+    <row r="207" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B207" s="3"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -3708,7 +3771,7 @@
       <c r="M207" s="1"/>
       <c r="N207" s="13"/>
     </row>
-    <row r="208" spans="2:14">
+    <row r="208" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B208" s="3"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -3723,7 +3786,7 @@
       <c r="M208" s="1"/>
       <c r="N208" s="13"/>
     </row>
-    <row r="209" spans="2:14">
+    <row r="209" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B209" s="3"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -3738,7 +3801,7 @@
       <c r="M209" s="1"/>
       <c r="N209" s="13"/>
     </row>
-    <row r="210" spans="2:14">
+    <row r="210" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B210" s="3"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -3753,7 +3816,7 @@
       <c r="M210" s="1"/>
       <c r="N210" s="13"/>
     </row>
-    <row r="211" spans="2:14">
+    <row r="211" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B211" s="3"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -3768,7 +3831,7 @@
       <c r="M211" s="1"/>
       <c r="N211" s="13"/>
     </row>
-    <row r="212" spans="2:14">
+    <row r="212" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B212" s="3"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -3783,7 +3846,7 @@
       <c r="M212" s="1"/>
       <c r="N212" s="13"/>
     </row>
-    <row r="213" spans="2:14">
+    <row r="213" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B213" s="3"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -3798,7 +3861,7 @@
       <c r="M213" s="1"/>
       <c r="N213" s="13"/>
     </row>
-    <row r="214" spans="2:14">
+    <row r="214" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B214" s="3"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -3813,7 +3876,7 @@
       <c r="M214" s="1"/>
       <c r="N214" s="13"/>
     </row>
-    <row r="215" spans="2:14">
+    <row r="215" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B215" s="3"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -3828,7 +3891,7 @@
       <c r="M215" s="1"/>
       <c r="N215" s="13"/>
     </row>
-    <row r="216" spans="2:14">
+    <row r="216" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B216" s="3"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -3843,7 +3906,7 @@
       <c r="M216" s="1"/>
       <c r="N216" s="13"/>
     </row>
-    <row r="217" spans="2:14">
+    <row r="217" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B217" s="3"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -3858,7 +3921,7 @@
       <c r="M217" s="1"/>
       <c r="N217" s="13"/>
     </row>
-    <row r="218" spans="2:14">
+    <row r="218" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B218" s="3"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -3873,7 +3936,7 @@
       <c r="M218" s="1"/>
       <c r="N218" s="13"/>
     </row>
-    <row r="219" spans="2:14">
+    <row r="219" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B219" s="3"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
@@ -3888,7 +3951,7 @@
       <c r="M219" s="1"/>
       <c r="N219" s="13"/>
     </row>
-    <row r="220" spans="2:14">
+    <row r="220" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B220" s="3"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
@@ -3903,7 +3966,7 @@
       <c r="M220" s="1"/>
       <c r="N220" s="13"/>
     </row>
-    <row r="221" spans="2:14">
+    <row r="221" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B221" s="3"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
@@ -3918,7 +3981,7 @@
       <c r="M221" s="1"/>
       <c r="N221" s="13"/>
     </row>
-    <row r="222" spans="2:14">
+    <row r="222" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B222" s="3"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
@@ -3933,7 +3996,7 @@
       <c r="M222" s="1"/>
       <c r="N222" s="13"/>
     </row>
-    <row r="223" spans="2:14">
+    <row r="223" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B223" s="3"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
@@ -3948,7 +4011,7 @@
       <c r="M223" s="1"/>
       <c r="N223" s="13"/>
     </row>
-    <row r="224" spans="2:14">
+    <row r="224" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B224" s="3"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
@@ -3963,7 +4026,7 @@
       <c r="M224" s="1"/>
       <c r="N224" s="13"/>
     </row>
-    <row r="225" spans="2:14">
+    <row r="225" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B225" s="3"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
@@ -3978,7 +4041,7 @@
       <c r="M225" s="1"/>
       <c r="N225" s="13"/>
     </row>
-    <row r="226" spans="2:14">
+    <row r="226" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B226" s="3"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -3993,7 +4056,7 @@
       <c r="M226" s="1"/>
       <c r="N226" s="13"/>
     </row>
-    <row r="227" spans="2:14">
+    <row r="227" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B227" s="3"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -4008,7 +4071,7 @@
       <c r="M227" s="1"/>
       <c r="N227" s="13"/>
     </row>
-    <row r="228" spans="2:14">
+    <row r="228" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B228" s="3"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -4023,7 +4086,7 @@
       <c r="M228" s="1"/>
       <c r="N228" s="13"/>
     </row>
-    <row r="229" spans="2:14">
+    <row r="229" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B229" s="3"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
@@ -4038,7 +4101,7 @@
       <c r="M229" s="1"/>
       <c r="N229" s="13"/>
     </row>
-    <row r="230" spans="2:14">
+    <row r="230" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B230" s="3"/>
       <c r="C230" s="1"/>
       <c r="D230" s="1"/>
@@ -4053,7 +4116,7 @@
       <c r="M230" s="1"/>
       <c r="N230" s="13"/>
     </row>
-    <row r="231" spans="2:14">
+    <row r="231" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B231" s="3"/>
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
@@ -4068,7 +4131,7 @@
       <c r="M231" s="1"/>
       <c r="N231" s="13"/>
     </row>
-    <row r="232" spans="2:14">
+    <row r="232" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B232" s="3"/>
       <c r="C232" s="1"/>
       <c r="D232" s="1"/>
@@ -4083,7 +4146,7 @@
       <c r="M232" s="1"/>
       <c r="N232" s="13"/>
     </row>
-    <row r="233" spans="2:14">
+    <row r="233" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B233" s="3"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
@@ -4098,7 +4161,7 @@
       <c r="M233" s="1"/>
       <c r="N233" s="13"/>
     </row>
-    <row r="234" spans="2:14">
+    <row r="234" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B234" s="3"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
@@ -4113,7 +4176,7 @@
       <c r="M234" s="1"/>
       <c r="N234" s="13"/>
     </row>
-    <row r="235" spans="2:14">
+    <row r="235" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B235" s="3"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
@@ -4128,7 +4191,7 @@
       <c r="M235" s="1"/>
       <c r="N235" s="13"/>
     </row>
-    <row r="236" spans="2:14">
+    <row r="236" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B236" s="3"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
@@ -4143,7 +4206,7 @@
       <c r="M236" s="1"/>
       <c r="N236" s="13"/>
     </row>
-    <row r="237" spans="2:14">
+    <row r="237" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B237" s="3"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
@@ -4158,7 +4221,7 @@
       <c r="M237" s="1"/>
       <c r="N237" s="13"/>
     </row>
-    <row r="238" spans="2:14">
+    <row r="238" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B238" s="3"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
@@ -4173,7 +4236,7 @@
       <c r="M238" s="1"/>
       <c r="N238" s="13"/>
     </row>
-    <row r="239" spans="2:14">
+    <row r="239" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B239" s="3"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
@@ -4188,7 +4251,7 @@
       <c r="M239" s="1"/>
       <c r="N239" s="13"/>
     </row>
-    <row r="240" spans="2:14">
+    <row r="240" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B240" s="3"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -4203,7 +4266,7 @@
       <c r="M240" s="1"/>
       <c r="N240" s="13"/>
     </row>
-    <row r="241" spans="2:14">
+    <row r="241" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B241" s="3"/>
       <c r="C241" s="1"/>
       <c r="D241" s="1"/>
@@ -4218,7 +4281,7 @@
       <c r="M241" s="1"/>
       <c r="N241" s="13"/>
     </row>
-    <row r="242" spans="2:14">
+    <row r="242" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B242" s="3"/>
       <c r="C242" s="1"/>
       <c r="D242" s="1"/>
@@ -4233,7 +4296,7 @@
       <c r="M242" s="1"/>
       <c r="N242" s="13"/>
     </row>
-    <row r="243" spans="2:14">
+    <row r="243" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B243" s="3"/>
       <c r="C243" s="1"/>
       <c r="D243" s="1"/>
@@ -4248,7 +4311,7 @@
       <c r="M243" s="1"/>
       <c r="N243" s="13"/>
     </row>
-    <row r="244" spans="2:14">
+    <row r="244" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B244" s="3"/>
       <c r="C244" s="1"/>
       <c r="D244" s="1"/>
@@ -4263,7 +4326,7 @@
       <c r="M244" s="1"/>
       <c r="N244" s="13"/>
     </row>
-    <row r="245" spans="2:14">
+    <row r="245" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B245" s="3"/>
       <c r="C245" s="1"/>
       <c r="D245" s="1"/>
@@ -4278,7 +4341,7 @@
       <c r="M245" s="1"/>
       <c r="N245" s="13"/>
     </row>
-    <row r="246" spans="2:14">
+    <row r="246" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B246" s="3"/>
       <c r="C246" s="1"/>
       <c r="D246" s="1"/>
@@ -4293,7 +4356,7 @@
       <c r="M246" s="1"/>
       <c r="N246" s="13"/>
     </row>
-    <row r="247" spans="2:14">
+    <row r="247" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B247" s="3"/>
       <c r="C247" s="1"/>
       <c r="D247" s="1"/>
@@ -4308,7 +4371,7 @@
       <c r="M247" s="1"/>
       <c r="N247" s="13"/>
     </row>
-    <row r="248" spans="2:14">
+    <row r="248" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B248" s="3"/>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -4323,7 +4386,7 @@
       <c r="M248" s="1"/>
       <c r="N248" s="13"/>
     </row>
-    <row r="249" spans="2:14">
+    <row r="249" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B249" s="3"/>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -4338,7 +4401,7 @@
       <c r="M249" s="1"/>
       <c r="N249" s="13"/>
     </row>
-    <row r="250" spans="2:14">
+    <row r="250" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B250" s="3"/>
       <c r="C250" s="1"/>
       <c r="D250" s="1"/>
@@ -4353,7 +4416,7 @@
       <c r="M250" s="1"/>
       <c r="N250" s="13"/>
     </row>
-    <row r="251" spans="2:14">
+    <row r="251" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B251" s="3"/>
       <c r="C251" s="1"/>
       <c r="D251" s="1"/>
@@ -4368,7 +4431,7 @@
       <c r="M251" s="1"/>
       <c r="N251" s="13"/>
     </row>
-    <row r="252" spans="2:14">
+    <row r="252" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B252" s="3"/>
       <c r="C252" s="1"/>
       <c r="D252" s="1"/>
@@ -4383,7 +4446,7 @@
       <c r="M252" s="1"/>
       <c r="N252" s="13"/>
     </row>
-    <row r="253" spans="2:14">
+    <row r="253" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B253" s="3"/>
       <c r="C253" s="1"/>
       <c r="D253" s="1"/>
@@ -4398,7 +4461,7 @@
       <c r="M253" s="1"/>
       <c r="N253" s="13"/>
     </row>
-    <row r="254" spans="2:14">
+    <row r="254" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B254" s="3"/>
       <c r="C254" s="1"/>
       <c r="D254" s="1"/>
@@ -4413,7 +4476,7 @@
       <c r="M254" s="1"/>
       <c r="N254" s="13"/>
     </row>
-    <row r="255" spans="2:14">
+    <row r="255" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B255" s="3"/>
       <c r="C255" s="1"/>
       <c r="D255" s="1"/>
@@ -4428,7 +4491,7 @@
       <c r="M255" s="1"/>
       <c r="N255" s="13"/>
     </row>
-    <row r="256" spans="2:14">
+    <row r="256" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B256" s="3"/>
       <c r="C256" s="1"/>
       <c r="D256" s="1"/>
@@ -4443,7 +4506,7 @@
       <c r="M256" s="1"/>
       <c r="N256" s="13"/>
     </row>
-    <row r="257" spans="2:14">
+    <row r="257" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B257" s="3"/>
       <c r="C257" s="1"/>
       <c r="D257" s="1"/>
@@ -4458,7 +4521,7 @@
       <c r="M257" s="1"/>
       <c r="N257" s="13"/>
     </row>
-    <row r="258" spans="2:14">
+    <row r="258" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B258" s="3"/>
       <c r="C258" s="1"/>
       <c r="D258" s="1"/>
@@ -4473,7 +4536,7 @@
       <c r="M258" s="1"/>
       <c r="N258" s="13"/>
     </row>
-    <row r="259" spans="2:14">
+    <row r="259" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B259" s="3"/>
       <c r="C259" s="1"/>
       <c r="D259" s="1"/>
@@ -4488,7 +4551,7 @@
       <c r="M259" s="1"/>
       <c r="N259" s="13"/>
     </row>
-    <row r="260" spans="2:14">
+    <row r="260" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B260" s="3"/>
       <c r="C260" s="1"/>
       <c r="D260" s="1"/>
@@ -4503,7 +4566,7 @@
       <c r="M260" s="1"/>
       <c r="N260" s="13"/>
     </row>
-    <row r="261" spans="2:14">
+    <row r="261" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B261" s="3"/>
       <c r="C261" s="1"/>
       <c r="D261" s="1"/>
@@ -4518,7 +4581,7 @@
       <c r="M261" s="1"/>
       <c r="N261" s="13"/>
     </row>
-    <row r="262" spans="2:14">
+    <row r="262" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B262" s="3"/>
       <c r="C262" s="1"/>
       <c r="D262" s="1"/>
@@ -4533,7 +4596,7 @@
       <c r="M262" s="1"/>
       <c r="N262" s="13"/>
     </row>
-    <row r="263" spans="2:14">
+    <row r="263" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B263" s="3"/>
       <c r="C263" s="1"/>
       <c r="D263" s="1"/>
@@ -4548,7 +4611,7 @@
       <c r="M263" s="1"/>
       <c r="N263" s="13"/>
     </row>
-    <row r="264" spans="2:14">
+    <row r="264" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B264" s="3"/>
       <c r="C264" s="1"/>
       <c r="D264" s="1"/>
@@ -4563,7 +4626,7 @@
       <c r="M264" s="1"/>
       <c r="N264" s="13"/>
     </row>
-    <row r="265" spans="2:14">
+    <row r="265" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B265" s="3"/>
       <c r="C265" s="1"/>
       <c r="D265" s="1"/>
@@ -4578,7 +4641,7 @@
       <c r="M265" s="1"/>
       <c r="N265" s="13"/>
     </row>
-    <row r="266" spans="2:14">
+    <row r="266" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B266" s="3"/>
       <c r="C266" s="1"/>
       <c r="D266" s="1"/>
@@ -4593,7 +4656,7 @@
       <c r="M266" s="1"/>
       <c r="N266" s="13"/>
     </row>
-    <row r="267" spans="2:14">
+    <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B267" s="3"/>
       <c r="C267" s="1"/>
       <c r="D267" s="1"/>
@@ -4608,7 +4671,7 @@
       <c r="M267" s="1"/>
       <c r="N267" s="13"/>
     </row>
-    <row r="268" spans="2:14">
+    <row r="268" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B268" s="3"/>
       <c r="C268" s="1"/>
       <c r="D268" s="1"/>
@@ -4623,7 +4686,7 @@
       <c r="M268" s="1"/>
       <c r="N268" s="13"/>
     </row>
-    <row r="269" spans="2:14">
+    <row r="269" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B269" s="3"/>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
@@ -4638,7 +4701,7 @@
       <c r="M269" s="1"/>
       <c r="N269" s="13"/>
     </row>
-    <row r="270" spans="2:14">
+    <row r="270" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B270" s="3"/>
       <c r="C270" s="1"/>
       <c r="D270" s="1"/>
@@ -4653,7 +4716,7 @@
       <c r="M270" s="1"/>
       <c r="N270" s="13"/>
     </row>
-    <row r="271" spans="2:14">
+    <row r="271" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B271" s="3"/>
       <c r="C271" s="1"/>
       <c r="D271" s="1"/>
@@ -4668,7 +4731,7 @@
       <c r="M271" s="1"/>
       <c r="N271" s="13"/>
     </row>
-    <row r="272" spans="2:14">
+    <row r="272" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B272" s="3"/>
       <c r="C272" s="1"/>
       <c r="D272" s="1"/>
@@ -4683,7 +4746,7 @@
       <c r="M272" s="1"/>
       <c r="N272" s="13"/>
     </row>
-    <row r="273" spans="2:14">
+    <row r="273" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B273" s="3"/>
       <c r="C273" s="1"/>
       <c r="D273" s="1"/>
@@ -4698,7 +4761,7 @@
       <c r="M273" s="1"/>
       <c r="N273" s="13"/>
     </row>
-    <row r="274" spans="2:14">
+    <row r="274" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B274" s="3"/>
       <c r="C274" s="1"/>
       <c r="D274" s="1"/>
@@ -4713,7 +4776,7 @@
       <c r="M274" s="1"/>
       <c r="N274" s="13"/>
     </row>
-    <row r="275" spans="2:14">
+    <row r="275" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B275" s="3"/>
       <c r="C275" s="1"/>
       <c r="D275" s="1"/>
@@ -4728,7 +4791,7 @@
       <c r="M275" s="1"/>
       <c r="N275" s="13"/>
     </row>
-    <row r="276" spans="2:14">
+    <row r="276" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B276" s="3"/>
       <c r="C276" s="1"/>
       <c r="D276" s="1"/>
@@ -4743,7 +4806,7 @@
       <c r="M276" s="1"/>
       <c r="N276" s="13"/>
     </row>
-    <row r="277" spans="2:14">
+    <row r="277" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B277" s="3"/>
       <c r="C277" s="1"/>
       <c r="D277" s="1"/>
@@ -4758,7 +4821,7 @@
       <c r="M277" s="1"/>
       <c r="N277" s="13"/>
     </row>
-    <row r="278" spans="2:14">
+    <row r="278" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B278" s="3"/>
       <c r="C278" s="1"/>
       <c r="D278" s="1"/>
@@ -4773,7 +4836,7 @@
       <c r="M278" s="1"/>
       <c r="N278" s="13"/>
     </row>
-    <row r="279" spans="2:14">
+    <row r="279" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B279" s="3"/>
       <c r="C279" s="1"/>
       <c r="D279" s="1"/>
@@ -4788,7 +4851,7 @@
       <c r="M279" s="1"/>
       <c r="N279" s="13"/>
     </row>
-    <row r="280" spans="2:14">
+    <row r="280" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B280" s="3"/>
       <c r="C280" s="1"/>
       <c r="D280" s="1"/>
@@ -4803,7 +4866,7 @@
       <c r="M280" s="1"/>
       <c r="N280" s="13"/>
     </row>
-    <row r="281" spans="2:14">
+    <row r="281" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B281" s="3"/>
       <c r="C281" s="1"/>
       <c r="D281" s="1"/>
@@ -4818,7 +4881,7 @@
       <c r="M281" s="1"/>
       <c r="N281" s="13"/>
     </row>
-    <row r="282" spans="2:14">
+    <row r="282" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B282" s="3"/>
       <c r="C282" s="1"/>
       <c r="D282" s="1"/>
@@ -4833,7 +4896,7 @@
       <c r="M282" s="1"/>
       <c r="N282" s="13"/>
     </row>
-    <row r="283" spans="2:14">
+    <row r="283" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B283" s="3"/>
       <c r="C283" s="1"/>
       <c r="D283" s="1"/>
@@ -4848,7 +4911,7 @@
       <c r="M283" s="1"/>
       <c r="N283" s="13"/>
     </row>
-    <row r="284" spans="2:14">
+    <row r="284" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B284" s="3"/>
       <c r="C284" s="1"/>
       <c r="D284" s="1"/>
@@ -4863,7 +4926,7 @@
       <c r="M284" s="1"/>
       <c r="N284" s="13"/>
     </row>
-    <row r="285" spans="2:14">
+    <row r="285" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B285" s="3"/>
       <c r="C285" s="1"/>
       <c r="D285" s="1"/>
@@ -4878,7 +4941,7 @@
       <c r="M285" s="1"/>
       <c r="N285" s="13"/>
     </row>
-    <row r="286" spans="2:14">
+    <row r="286" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B286" s="3"/>
       <c r="C286" s="1"/>
       <c r="D286" s="1"/>
@@ -4893,7 +4956,7 @@
       <c r="M286" s="1"/>
       <c r="N286" s="13"/>
     </row>
-    <row r="287" spans="2:14">
+    <row r="287" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B287" s="3"/>
       <c r="C287" s="1"/>
       <c r="D287" s="1"/>
@@ -4908,7 +4971,7 @@
       <c r="M287" s="1"/>
       <c r="N287" s="13"/>
     </row>
-    <row r="288" spans="2:14">
+    <row r="288" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B288" s="3"/>
       <c r="C288" s="1"/>
       <c r="D288" s="1"/>
@@ -4923,7 +4986,7 @@
       <c r="M288" s="1"/>
       <c r="N288" s="13"/>
     </row>
-    <row r="289" spans="2:14">
+    <row r="289" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B289" s="3"/>
       <c r="C289" s="1"/>
       <c r="D289" s="1"/>
@@ -4938,7 +5001,7 @@
       <c r="M289" s="1"/>
       <c r="N289" s="13"/>
     </row>
-    <row r="290" spans="2:14">
+    <row r="290" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B290" s="3"/>
       <c r="C290" s="1"/>
       <c r="D290" s="1"/>
@@ -4953,7 +5016,7 @@
       <c r="M290" s="1"/>
       <c r="N290" s="13"/>
     </row>
-    <row r="291" spans="2:14">
+    <row r="291" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B291" s="3"/>
       <c r="C291" s="1"/>
       <c r="D291" s="1"/>
@@ -4968,7 +5031,7 @@
       <c r="M291" s="1"/>
       <c r="N291" s="13"/>
     </row>
-    <row r="292" spans="2:14">
+    <row r="292" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B292" s="3"/>
       <c r="C292" s="1"/>
       <c r="D292" s="1"/>
@@ -4983,7 +5046,7 @@
       <c r="M292" s="1"/>
       <c r="N292" s="13"/>
     </row>
-    <row r="293" spans="2:14">
+    <row r="293" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B293" s="3"/>
       <c r="C293" s="1"/>
       <c r="D293" s="1"/>
@@ -4998,7 +5061,7 @@
       <c r="M293" s="1"/>
       <c r="N293" s="13"/>
     </row>
-    <row r="294" spans="2:14">
+    <row r="294" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B294" s="3"/>
       <c r="C294" s="1"/>
       <c r="D294" s="1"/>
@@ -5013,7 +5076,7 @@
       <c r="M294" s="1"/>
       <c r="N294" s="13"/>
     </row>
-    <row r="295" spans="2:14">
+    <row r="295" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B295" s="3"/>
       <c r="C295" s="1"/>
       <c r="D295" s="1"/>
@@ -5028,7 +5091,7 @@
       <c r="M295" s="1"/>
       <c r="N295" s="13"/>
     </row>
-    <row r="296" spans="2:14">
+    <row r="296" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B296" s="3"/>
       <c r="C296" s="1"/>
       <c r="D296" s="1"/>
@@ -5043,7 +5106,7 @@
       <c r="M296" s="1"/>
       <c r="N296" s="13"/>
     </row>
-    <row r="297" spans="2:14">
+    <row r="297" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B297" s="3"/>
       <c r="C297" s="1"/>
       <c r="D297" s="1"/>
@@ -5058,7 +5121,7 @@
       <c r="M297" s="1"/>
       <c r="N297" s="13"/>
     </row>
-    <row r="298" spans="2:14">
+    <row r="298" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B298" s="3"/>
       <c r="C298" s="1"/>
       <c r="D298" s="1"/>
@@ -5073,7 +5136,7 @@
       <c r="M298" s="1"/>
       <c r="N298" s="13"/>
     </row>
-    <row r="299" spans="2:14">
+    <row r="299" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B299" s="3"/>
       <c r="C299" s="1"/>
       <c r="D299" s="1"/>
@@ -5088,7 +5151,7 @@
       <c r="M299" s="1"/>
       <c r="N299" s="13"/>
     </row>
-    <row r="300" spans="2:14">
+    <row r="300" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B300" s="3"/>
       <c r="C300" s="1"/>
       <c r="D300" s="1"/>
@@ -5103,7 +5166,7 @@
       <c r="M300" s="1"/>
       <c r="N300" s="13"/>
     </row>
-    <row r="301" spans="2:14">
+    <row r="301" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B301" s="3"/>
       <c r="C301" s="1"/>
       <c r="D301" s="1"/>
@@ -5118,7 +5181,7 @@
       <c r="M301" s="1"/>
       <c r="N301" s="13"/>
     </row>
-    <row r="302" spans="2:14">
+    <row r="302" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B302" s="3"/>
       <c r="C302" s="1"/>
       <c r="D302" s="1"/>
@@ -5133,7 +5196,7 @@
       <c r="M302" s="1"/>
       <c r="N302" s="13"/>
     </row>
-    <row r="303" spans="2:14">
+    <row r="303" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B303" s="3"/>
       <c r="C303" s="1"/>
       <c r="D303" s="1"/>
@@ -5148,7 +5211,7 @@
       <c r="M303" s="1"/>
       <c r="N303" s="13"/>
     </row>
-    <row r="304" spans="2:14">
+    <row r="304" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B304" s="3"/>
       <c r="C304" s="1"/>
       <c r="D304" s="1"/>
@@ -5163,7 +5226,7 @@
       <c r="M304" s="1"/>
       <c r="N304" s="13"/>
     </row>
-    <row r="305" spans="2:14">
+    <row r="305" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B305" s="3"/>
       <c r="C305" s="1"/>
       <c r="D305" s="1"/>
@@ -5178,7 +5241,7 @@
       <c r="M305" s="1"/>
       <c r="N305" s="13"/>
     </row>
-    <row r="306" spans="2:14">
+    <row r="306" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B306" s="3"/>
       <c r="C306" s="1"/>
       <c r="D306" s="1"/>
@@ -5193,7 +5256,7 @@
       <c r="M306" s="1"/>
       <c r="N306" s="13"/>
     </row>
-    <row r="307" spans="2:14">
+    <row r="307" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B307" s="3"/>
       <c r="C307" s="1"/>
       <c r="D307" s="1"/>
@@ -5208,7 +5271,7 @@
       <c r="M307" s="1"/>
       <c r="N307" s="13"/>
     </row>
-    <row r="308" spans="2:14">
+    <row r="308" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B308" s="3"/>
       <c r="C308" s="1"/>
       <c r="D308" s="1"/>
@@ -5223,7 +5286,7 @@
       <c r="M308" s="1"/>
       <c r="N308" s="13"/>
     </row>
-    <row r="309" spans="2:14">
+    <row r="309" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B309" s="3"/>
       <c r="C309" s="1"/>
       <c r="D309" s="1"/>
@@ -5238,7 +5301,7 @@
       <c r="M309" s="1"/>
       <c r="N309" s="13"/>
     </row>
-    <row r="310" spans="2:14">
+    <row r="310" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B310" s="3"/>
       <c r="C310" s="1"/>
       <c r="D310" s="1"/>
@@ -5253,7 +5316,7 @@
       <c r="M310" s="1"/>
       <c r="N310" s="13"/>
     </row>
-    <row r="311" spans="2:14">
+    <row r="311" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B311" s="3"/>
       <c r="C311" s="1"/>
       <c r="D311" s="1"/>
@@ -5268,7 +5331,7 @@
       <c r="M311" s="1"/>
       <c r="N311" s="13"/>
     </row>
-    <row r="312" spans="2:14">
+    <row r="312" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B312" s="3"/>
       <c r="C312" s="1"/>
       <c r="D312" s="1"/>
@@ -5283,7 +5346,7 @@
       <c r="M312" s="1"/>
       <c r="N312" s="13"/>
     </row>
-    <row r="313" spans="2:14">
+    <row r="313" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B313" s="3"/>
       <c r="C313" s="1"/>
       <c r="D313" s="1"/>
@@ -5298,7 +5361,7 @@
       <c r="M313" s="1"/>
       <c r="N313" s="13"/>
     </row>
-    <row r="314" spans="2:14">
+    <row r="314" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B314" s="3"/>
       <c r="C314" s="1"/>
       <c r="D314" s="1"/>
@@ -5313,7 +5376,7 @@
       <c r="M314" s="1"/>
       <c r="N314" s="13"/>
     </row>
-    <row r="315" spans="2:14">
+    <row r="315" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B315" s="3"/>
       <c r="C315" s="1"/>
       <c r="D315" s="1"/>
@@ -5328,7 +5391,7 @@
       <c r="M315" s="1"/>
       <c r="N315" s="13"/>
     </row>
-    <row r="316" spans="2:14">
+    <row r="316" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B316" s="3"/>
       <c r="C316" s="1"/>
       <c r="D316" s="1"/>
@@ -5343,7 +5406,7 @@
       <c r="M316" s="1"/>
       <c r="N316" s="13"/>
     </row>
-    <row r="317" spans="2:14">
+    <row r="317" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B317" s="3"/>
       <c r="C317" s="1"/>
       <c r="D317" s="1"/>
@@ -5358,7 +5421,7 @@
       <c r="M317" s="1"/>
       <c r="N317" s="13"/>
     </row>
-    <row r="318" spans="2:14">
+    <row r="318" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B318" s="3"/>
       <c r="C318" s="1"/>
       <c r="D318" s="1"/>
@@ -5373,7 +5436,7 @@
       <c r="M318" s="1"/>
       <c r="N318" s="13"/>
     </row>
-    <row r="319" spans="2:14">
+    <row r="319" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B319" s="3"/>
       <c r="C319" s="1"/>
       <c r="D319" s="1"/>
@@ -5388,7 +5451,7 @@
       <c r="M319" s="1"/>
       <c r="N319" s="13"/>
     </row>
-    <row r="320" spans="2:14">
+    <row r="320" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B320" s="3"/>
       <c r="C320" s="1"/>
       <c r="D320" s="1"/>
@@ -5403,7 +5466,7 @@
       <c r="M320" s="1"/>
       <c r="N320" s="13"/>
     </row>
-    <row r="321" spans="2:14">
+    <row r="321" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B321" s="3"/>
       <c r="C321" s="1"/>
       <c r="D321" s="1"/>
@@ -5418,7 +5481,7 @@
       <c r="M321" s="1"/>
       <c r="N321" s="13"/>
     </row>
-    <row r="322" spans="2:14">
+    <row r="322" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B322" s="3"/>
       <c r="C322" s="1"/>
       <c r="D322" s="1"/>
@@ -5433,7 +5496,7 @@
       <c r="M322" s="1"/>
       <c r="N322" s="13"/>
     </row>
-    <row r="323" spans="2:14">
+    <row r="323" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B323" s="3"/>
       <c r="C323" s="1"/>
       <c r="D323" s="1"/>
@@ -5448,7 +5511,7 @@
       <c r="M323" s="1"/>
       <c r="N323" s="13"/>
     </row>
-    <row r="324" spans="2:14">
+    <row r="324" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B324" s="3"/>
       <c r="C324" s="1"/>
       <c r="D324" s="1"/>
@@ -5463,7 +5526,7 @@
       <c r="M324" s="1"/>
       <c r="N324" s="13"/>
     </row>
-    <row r="325" spans="2:14">
+    <row r="325" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B325" s="3"/>
       <c r="C325" s="1"/>
       <c r="D325" s="1"/>
@@ -5478,7 +5541,7 @@
       <c r="M325" s="1"/>
       <c r="N325" s="13"/>
     </row>
-    <row r="326" spans="2:14">
+    <row r="326" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B326" s="3"/>
       <c r="C326" s="1"/>
       <c r="D326" s="1"/>
@@ -5493,7 +5556,7 @@
       <c r="M326" s="1"/>
       <c r="N326" s="13"/>
     </row>
-    <row r="327" spans="2:14">
+    <row r="327" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B327" s="3"/>
       <c r="C327" s="1"/>
       <c r="D327" s="1"/>
@@ -5508,7 +5571,7 @@
       <c r="M327" s="1"/>
       <c r="N327" s="13"/>
     </row>
-    <row r="328" spans="2:14">
+    <row r="328" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B328" s="3"/>
       <c r="C328" s="1"/>
       <c r="D328" s="1"/>
@@ -5523,7 +5586,7 @@
       <c r="M328" s="1"/>
       <c r="N328" s="13"/>
     </row>
-    <row r="329" spans="2:14">
+    <row r="329" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B329" s="3"/>
       <c r="C329" s="1"/>
       <c r="D329" s="1"/>
@@ -5538,7 +5601,7 @@
       <c r="M329" s="1"/>
       <c r="N329" s="13"/>
     </row>
-    <row r="330" spans="2:14">
+    <row r="330" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B330" s="3"/>
       <c r="C330" s="1"/>
       <c r="D330" s="1"/>
@@ -5553,7 +5616,7 @@
       <c r="M330" s="1"/>
       <c r="N330" s="13"/>
     </row>
-    <row r="331" spans="2:14">
+    <row r="331" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B331" s="3"/>
       <c r="C331" s="1"/>
       <c r="D331" s="1"/>
@@ -5568,7 +5631,7 @@
       <c r="M331" s="1"/>
       <c r="N331" s="13"/>
     </row>
-    <row r="332" spans="2:14">
+    <row r="332" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B332" s="3"/>
       <c r="C332" s="1"/>
       <c r="D332" s="1"/>
@@ -5583,7 +5646,7 @@
       <c r="M332" s="1"/>
       <c r="N332" s="13"/>
     </row>
-    <row r="333" spans="2:14">
+    <row r="333" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B333" s="3"/>
       <c r="C333" s="1"/>
       <c r="D333" s="1"/>
@@ -5598,7 +5661,7 @@
       <c r="M333" s="1"/>
       <c r="N333" s="13"/>
     </row>
-    <row r="334" spans="2:14">
+    <row r="334" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B334" s="3"/>
       <c r="C334" s="1"/>
       <c r="D334" s="1"/>
@@ -5613,7 +5676,7 @@
       <c r="M334" s="1"/>
       <c r="N334" s="13"/>
     </row>
-    <row r="335" spans="2:14">
+    <row r="335" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B335" s="3"/>
       <c r="C335" s="1"/>
       <c r="D335" s="1"/>
@@ -5628,7 +5691,7 @@
       <c r="M335" s="1"/>
       <c r="N335" s="13"/>
     </row>
-    <row r="336" spans="2:14">
+    <row r="336" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B336" s="3"/>
       <c r="C336" s="1"/>
       <c r="D336" s="1"/>
@@ -5643,7 +5706,7 @@
       <c r="M336" s="1"/>
       <c r="N336" s="13"/>
     </row>
-    <row r="337" spans="2:14">
+    <row r="337" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B337" s="3"/>
       <c r="C337" s="1"/>
       <c r="D337" s="1"/>
@@ -5658,7 +5721,7 @@
       <c r="M337" s="1"/>
       <c r="N337" s="13"/>
     </row>
-    <row r="338" spans="2:14">
+    <row r="338" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B338" s="3"/>
       <c r="C338" s="1"/>
       <c r="D338" s="1"/>
@@ -5673,7 +5736,7 @@
       <c r="M338" s="1"/>
       <c r="N338" s="13"/>
     </row>
-    <row r="339" spans="2:14">
+    <row r="339" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B339" s="3"/>
       <c r="C339" s="1"/>
       <c r="D339" s="1"/>
@@ -5688,7 +5751,7 @@
       <c r="M339" s="1"/>
       <c r="N339" s="13"/>
     </row>
-    <row r="340" spans="2:14">
+    <row r="340" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B340" s="3"/>
       <c r="C340" s="1"/>
       <c r="D340" s="1"/>
@@ -5703,7 +5766,7 @@
       <c r="M340" s="1"/>
       <c r="N340" s="13"/>
     </row>
-    <row r="341" spans="2:14">
+    <row r="341" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B341" s="3"/>
       <c r="C341" s="1"/>
       <c r="D341" s="1"/>
@@ -5718,7 +5781,7 @@
       <c r="M341" s="1"/>
       <c r="N341" s="13"/>
     </row>
-    <row r="342" spans="2:14">
+    <row r="342" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B342" s="3"/>
       <c r="C342" s="1"/>
       <c r="D342" s="1"/>
@@ -5733,7 +5796,7 @@
       <c r="M342" s="1"/>
       <c r="N342" s="13"/>
     </row>
-    <row r="343" spans="2:14">
+    <row r="343" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B343" s="3"/>
       <c r="C343" s="1"/>
       <c r="D343" s="1"/>
@@ -5748,7 +5811,7 @@
       <c r="M343" s="1"/>
       <c r="N343" s="13"/>
     </row>
-    <row r="344" spans="2:14">
+    <row r="344" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B344" s="3"/>
       <c r="C344" s="1"/>
       <c r="D344" s="1"/>
@@ -5763,7 +5826,7 @@
       <c r="M344" s="1"/>
       <c r="N344" s="13"/>
     </row>
-    <row r="345" spans="2:14">
+    <row r="345" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B345" s="3"/>
       <c r="C345" s="1"/>
       <c r="D345" s="1"/>
@@ -5778,7 +5841,7 @@
       <c r="M345" s="1"/>
       <c r="N345" s="13"/>
     </row>
-    <row r="346" spans="2:14">
+    <row r="346" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B346" s="3"/>
       <c r="C346" s="1"/>
       <c r="D346" s="1"/>
@@ -5793,7 +5856,7 @@
       <c r="M346" s="1"/>
       <c r="N346" s="13"/>
     </row>
-    <row r="347" spans="2:14">
+    <row r="347" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B347" s="3"/>
       <c r="C347" s="1"/>
       <c r="D347" s="1"/>
@@ -5808,7 +5871,7 @@
       <c r="M347" s="1"/>
       <c r="N347" s="13"/>
     </row>
-    <row r="348" spans="2:14">
+    <row r="348" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B348" s="3"/>
       <c r="C348" s="1"/>
       <c r="D348" s="1"/>
@@ -5823,7 +5886,7 @@
       <c r="M348" s="1"/>
       <c r="N348" s="13"/>
     </row>
-    <row r="349" spans="2:14">
+    <row r="349" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B349" s="3"/>
       <c r="C349" s="1"/>
       <c r="D349" s="1"/>
@@ -5838,7 +5901,7 @@
       <c r="M349" s="1"/>
       <c r="N349" s="13"/>
     </row>
-    <row r="350" spans="2:14">
+    <row r="350" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B350" s="3"/>
       <c r="C350" s="1"/>
       <c r="D350" s="1"/>
@@ -5853,7 +5916,7 @@
       <c r="M350" s="1"/>
       <c r="N350" s="13"/>
     </row>
-    <row r="351" spans="2:14">
+    <row r="351" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B351" s="3"/>
       <c r="C351" s="1"/>
       <c r="D351" s="1"/>
@@ -5868,7 +5931,7 @@
       <c r="M351" s="1"/>
       <c r="N351" s="13"/>
     </row>
-    <row r="352" spans="2:14">
+    <row r="352" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B352" s="3"/>
       <c r="C352" s="1"/>
       <c r="D352" s="1"/>
@@ -5883,7 +5946,7 @@
       <c r="M352" s="1"/>
       <c r="N352" s="13"/>
     </row>
-    <row r="353" spans="2:14">
+    <row r="353" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B353" s="3"/>
       <c r="C353" s="1"/>
       <c r="D353" s="1"/>
@@ -5898,7 +5961,7 @@
       <c r="M353" s="1"/>
       <c r="N353" s="13"/>
     </row>
-    <row r="354" spans="2:14">
+    <row r="354" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B354" s="3"/>
       <c r="C354" s="1"/>
       <c r="D354" s="1"/>
@@ -5913,7 +5976,7 @@
       <c r="M354" s="1"/>
       <c r="N354" s="13"/>
     </row>
-    <row r="355" spans="2:14">
+    <row r="355" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B355" s="3"/>
       <c r="C355" s="1"/>
       <c r="D355" s="1"/>
@@ -5928,7 +5991,7 @@
       <c r="M355" s="1"/>
       <c r="N355" s="13"/>
     </row>
-    <row r="356" spans="2:14">
+    <row r="356" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B356" s="3"/>
       <c r="C356" s="1"/>
       <c r="D356" s="1"/>
@@ -5943,7 +6006,7 @@
       <c r="M356" s="1"/>
       <c r="N356" s="13"/>
     </row>
-    <row r="357" spans="2:14">
+    <row r="357" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B357" s="3"/>
       <c r="C357" s="1"/>
       <c r="D357" s="1"/>
@@ -5958,7 +6021,7 @@
       <c r="M357" s="1"/>
       <c r="N357" s="13"/>
     </row>
-    <row r="358" spans="2:14">
+    <row r="358" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B358" s="3"/>
       <c r="C358" s="1"/>
       <c r="D358" s="1"/>
@@ -5973,7 +6036,7 @@
       <c r="M358" s="1"/>
       <c r="N358" s="13"/>
     </row>
-    <row r="359" spans="2:14">
+    <row r="359" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B359" s="3"/>
       <c r="C359" s="1"/>
       <c r="D359" s="1"/>
@@ -5988,7 +6051,7 @@
       <c r="M359" s="1"/>
       <c r="N359" s="13"/>
     </row>
-    <row r="360" spans="2:14">
+    <row r="360" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B360" s="3"/>
       <c r="C360" s="1"/>
       <c r="D360" s="1"/>
@@ -6003,7 +6066,7 @@
       <c r="M360" s="1"/>
       <c r="N360" s="13"/>
     </row>
-    <row r="361" spans="2:14">
+    <row r="361" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B361" s="3"/>
       <c r="C361" s="1"/>
       <c r="D361" s="1"/>
@@ -6018,7 +6081,7 @@
       <c r="M361" s="1"/>
       <c r="N361" s="13"/>
     </row>
-    <row r="362" spans="2:14">
+    <row r="362" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B362" s="3"/>
       <c r="C362" s="1"/>
       <c r="D362" s="1"/>
@@ -6033,7 +6096,7 @@
       <c r="M362" s="1"/>
       <c r="N362" s="13"/>
     </row>
-    <row r="363" spans="2:14">
+    <row r="363" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B363" s="3"/>
       <c r="C363" s="1"/>
       <c r="D363" s="1"/>
@@ -6048,7 +6111,7 @@
       <c r="M363" s="1"/>
       <c r="N363" s="13"/>
     </row>
-    <row r="364" spans="2:14">
+    <row r="364" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B364" s="3"/>
       <c r="C364" s="1"/>
       <c r="D364" s="1"/>
@@ -6063,7 +6126,7 @@
       <c r="M364" s="1"/>
       <c r="N364" s="13"/>
     </row>
-    <row r="365" spans="2:14">
+    <row r="365" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B365" s="3"/>
       <c r="C365" s="1"/>
       <c r="D365" s="1"/>
@@ -6078,7 +6141,7 @@
       <c r="M365" s="1"/>
       <c r="N365" s="13"/>
     </row>
-    <row r="366" spans="2:14">
+    <row r="366" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B366" s="3"/>
       <c r="C366" s="1"/>
       <c r="D366" s="1"/>
@@ -6093,7 +6156,7 @@
       <c r="M366" s="1"/>
       <c r="N366" s="13"/>
     </row>
-    <row r="367" spans="2:14">
+    <row r="367" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B367" s="3"/>
       <c r="C367" s="1"/>
       <c r="D367" s="1"/>
@@ -6108,7 +6171,7 @@
       <c r="M367" s="1"/>
       <c r="N367" s="13"/>
     </row>
-    <row r="368" spans="2:14">
+    <row r="368" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B368" s="3"/>
       <c r="C368" s="1"/>
       <c r="D368" s="1"/>
@@ -6123,7 +6186,7 @@
       <c r="M368" s="1"/>
       <c r="N368" s="13"/>
     </row>
-    <row r="369" spans="2:14">
+    <row r="369" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B369" s="3"/>
       <c r="C369" s="1"/>
       <c r="D369" s="1"/>
@@ -6138,7 +6201,7 @@
       <c r="M369" s="1"/>
       <c r="N369" s="13"/>
     </row>
-    <row r="370" spans="2:14">
+    <row r="370" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B370" s="3"/>
       <c r="C370" s="1"/>
       <c r="D370" s="1"/>
@@ -6153,7 +6216,7 @@
       <c r="M370" s="1"/>
       <c r="N370" s="13"/>
     </row>
-    <row r="371" spans="2:14">
+    <row r="371" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B371" s="3"/>
       <c r="C371" s="1"/>
       <c r="D371" s="1"/>
@@ -6168,7 +6231,7 @@
       <c r="M371" s="1"/>
       <c r="N371" s="13"/>
     </row>
-    <row r="372" spans="2:14">
+    <row r="372" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B372" s="3"/>
       <c r="C372" s="1"/>
       <c r="D372" s="1"/>
@@ -6183,7 +6246,7 @@
       <c r="M372" s="1"/>
       <c r="N372" s="13"/>
     </row>
-    <row r="373" spans="2:14">
+    <row r="373" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B373" s="3"/>
       <c r="C373" s="1"/>
       <c r="D373" s="1"/>
@@ -6198,7 +6261,7 @@
       <c r="M373" s="1"/>
       <c r="N373" s="13"/>
     </row>
-    <row r="374" spans="2:14">
+    <row r="374" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B374" s="3"/>
       <c r="C374" s="1"/>
       <c r="D374" s="1"/>
@@ -6213,7 +6276,7 @@
       <c r="M374" s="1"/>
       <c r="N374" s="13"/>
     </row>
-    <row r="375" spans="2:14">
+    <row r="375" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B375" s="3"/>
       <c r="C375" s="1"/>
       <c r="D375" s="1"/>
@@ -6228,7 +6291,7 @@
       <c r="M375" s="1"/>
       <c r="N375" s="13"/>
     </row>
-    <row r="376" spans="2:14">
+    <row r="376" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B376" s="3"/>
       <c r="C376" s="1"/>
       <c r="D376" s="1"/>
@@ -6243,7 +6306,7 @@
       <c r="M376" s="1"/>
       <c r="N376" s="13"/>
     </row>
-    <row r="377" spans="2:14">
+    <row r="377" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B377" s="3"/>
       <c r="C377" s="1"/>
       <c r="D377" s="1"/>
@@ -6258,7 +6321,7 @@
       <c r="M377" s="1"/>
       <c r="N377" s="14"/>
     </row>
-    <row r="378" spans="2:14">
+    <row r="378" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B378" s="3"/>
       <c r="C378" s="1"/>
       <c r="D378" s="1"/>
@@ -6273,7 +6336,7 @@
       <c r="M378" s="1"/>
       <c r="N378" s="14"/>
     </row>
-    <row r="379" spans="2:14">
+    <row r="379" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B379" s="3"/>
       <c r="C379" s="1"/>
       <c r="D379" s="1"/>
@@ -6288,7 +6351,7 @@
       <c r="M379" s="1"/>
       <c r="N379" s="14"/>
     </row>
-    <row r="380" spans="2:14">
+    <row r="380" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B380" s="3"/>
       <c r="C380" s="1"/>
       <c r="D380" s="1"/>
@@ -6303,7 +6366,7 @@
       <c r="M380" s="1"/>
       <c r="N380" s="14"/>
     </row>
-    <row r="381" spans="2:14">
+    <row r="381" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B381" s="3"/>
       <c r="C381" s="1"/>
       <c r="D381" s="1"/>
@@ -6318,7 +6381,7 @@
       <c r="M381" s="1"/>
       <c r="N381" s="14"/>
     </row>
-    <row r="382" spans="2:14">
+    <row r="382" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B382" s="3"/>
       <c r="C382" s="1"/>
       <c r="D382" s="1"/>
@@ -6333,7 +6396,7 @@
       <c r="M382" s="1"/>
       <c r="N382" s="14"/>
     </row>
-    <row r="383" spans="2:14">
+    <row r="383" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B383" s="3"/>
       <c r="C383" s="1"/>
       <c r="D383" s="1"/>
@@ -6348,7 +6411,7 @@
       <c r="M383" s="1"/>
       <c r="N383" s="14"/>
     </row>
-    <row r="384" spans="2:14">
+    <row r="384" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B384" s="3"/>
       <c r="C384" s="1"/>
       <c r="D384" s="1"/>
@@ -6363,717 +6426,718 @@
       <c r="M384" s="1"/>
       <c r="N384" s="14"/>
     </row>
-    <row r="385" spans="2:5">
+    <row r="385" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B385" s="3"/>
       <c r="C385" s="1"/>
       <c r="D385" s="1"/>
       <c r="E385" s="13"/>
     </row>
-    <row r="386" spans="2:5">
+    <row r="386" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B386" s="3"/>
       <c r="C386" s="1"/>
       <c r="D386" s="1"/>
       <c r="E386" s="13"/>
     </row>
-    <row r="387" spans="2:5">
+    <row r="387" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B387" s="3"/>
       <c r="C387" s="1"/>
       <c r="D387" s="1"/>
       <c r="E387" s="13"/>
     </row>
-    <row r="388" spans="2:5">
+    <row r="388" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B388" s="3"/>
       <c r="C388" s="1"/>
       <c r="D388" s="1"/>
       <c r="E388" s="13"/>
     </row>
-    <row r="389" spans="2:5">
+    <row r="389" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B389" s="3"/>
       <c r="C389" s="1"/>
       <c r="D389" s="1"/>
       <c r="E389" s="13"/>
     </row>
-    <row r="390" spans="2:5">
+    <row r="390" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B390" s="3"/>
       <c r="C390" s="1"/>
       <c r="D390" s="1"/>
       <c r="E390" s="13"/>
     </row>
-    <row r="391" spans="2:5">
+    <row r="391" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B391" s="3"/>
       <c r="C391" s="1"/>
       <c r="D391" s="1"/>
       <c r="E391" s="13"/>
     </row>
-    <row r="392" spans="2:5">
+    <row r="392" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B392" s="3"/>
       <c r="C392" s="1"/>
       <c r="D392" s="1"/>
       <c r="E392" s="13"/>
     </row>
-    <row r="393" spans="2:5">
+    <row r="393" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B393" s="3"/>
       <c r="C393" s="1"/>
       <c r="D393" s="1"/>
       <c r="E393" s="13"/>
     </row>
-    <row r="394" spans="2:5">
+    <row r="394" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B394" s="3"/>
       <c r="C394" s="1"/>
       <c r="D394" s="1"/>
       <c r="E394" s="13"/>
     </row>
-    <row r="395" spans="2:5">
+    <row r="395" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B395" s="3"/>
       <c r="C395" s="1"/>
       <c r="D395" s="1"/>
       <c r="E395" s="13"/>
     </row>
-    <row r="396" spans="2:5">
+    <row r="396" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B396" s="3"/>
       <c r="C396" s="1"/>
       <c r="D396" s="1"/>
       <c r="E396" s="13"/>
     </row>
-    <row r="397" spans="2:5">
+    <row r="397" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B397" s="3"/>
       <c r="C397" s="1"/>
       <c r="D397" s="1"/>
       <c r="E397" s="13"/>
     </row>
-    <row r="398" spans="2:5">
+    <row r="398" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B398" s="3"/>
       <c r="C398" s="1"/>
       <c r="D398" s="1"/>
       <c r="E398" s="13"/>
     </row>
-    <row r="399" spans="2:5">
+    <row r="399" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B399" s="3"/>
       <c r="C399" s="1"/>
       <c r="D399" s="1"/>
       <c r="E399" s="13"/>
     </row>
-    <row r="400" spans="2:5">
+    <row r="400" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B400" s="3"/>
       <c r="C400" s="1"/>
       <c r="D400" s="1"/>
       <c r="E400" s="13"/>
     </row>
-    <row r="401" spans="2:5">
+    <row r="401" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B401" s="3"/>
       <c r="C401" s="1"/>
       <c r="D401" s="1"/>
       <c r="E401" s="13"/>
     </row>
-    <row r="402" spans="2:5">
+    <row r="402" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B402" s="3"/>
       <c r="C402" s="1"/>
       <c r="D402" s="1"/>
       <c r="E402" s="13"/>
     </row>
-    <row r="403" spans="2:5">
+    <row r="403" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B403" s="3"/>
       <c r="C403" s="1"/>
       <c r="D403" s="1"/>
       <c r="E403" s="13"/>
     </row>
-    <row r="404" spans="2:5">
+    <row r="404" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B404" s="3"/>
       <c r="C404" s="1"/>
       <c r="D404" s="1"/>
       <c r="E404" s="13"/>
     </row>
-    <row r="405" spans="2:5">
+    <row r="405" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B405" s="3"/>
       <c r="C405" s="1"/>
       <c r="D405" s="1"/>
       <c r="E405" s="13"/>
     </row>
-    <row r="406" spans="2:5">
+    <row r="406" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B406" s="3"/>
       <c r="C406" s="1"/>
       <c r="D406" s="1"/>
       <c r="E406" s="13"/>
     </row>
-    <row r="407" spans="2:5">
+    <row r="407" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B407" s="3"/>
       <c r="C407" s="1"/>
       <c r="D407" s="1"/>
       <c r="E407" s="13"/>
     </row>
-    <row r="408" spans="2:5">
+    <row r="408" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B408" s="3"/>
       <c r="C408" s="1"/>
       <c r="D408" s="1"/>
       <c r="E408" s="13"/>
     </row>
-    <row r="409" spans="2:5">
+    <row r="409" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B409" s="3"/>
       <c r="C409" s="1"/>
       <c r="D409" s="1"/>
       <c r="E409" s="13"/>
     </row>
-    <row r="410" spans="2:5">
+    <row r="410" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B410" s="3"/>
       <c r="C410" s="1"/>
       <c r="D410" s="1"/>
       <c r="E410" s="13"/>
     </row>
-    <row r="411" spans="2:5">
+    <row r="411" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B411" s="3"/>
       <c r="C411" s="1"/>
       <c r="D411" s="1"/>
       <c r="E411" s="13"/>
     </row>
-    <row r="412" spans="2:5">
+    <row r="412" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B412" s="3"/>
       <c r="C412" s="1"/>
       <c r="D412" s="1"/>
       <c r="E412" s="13"/>
     </row>
-    <row r="413" spans="2:5">
+    <row r="413" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B413" s="3"/>
       <c r="C413" s="1"/>
       <c r="D413" s="1"/>
       <c r="E413" s="13"/>
     </row>
-    <row r="414" spans="2:5">
+    <row r="414" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B414" s="3"/>
       <c r="C414" s="1"/>
       <c r="D414" s="1"/>
       <c r="E414" s="13"/>
     </row>
-    <row r="415" spans="2:5">
+    <row r="415" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B415" s="3"/>
       <c r="C415" s="1"/>
       <c r="D415" s="1"/>
       <c r="E415" s="13"/>
     </row>
-    <row r="416" spans="2:5">
+    <row r="416" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B416" s="3"/>
       <c r="C416" s="1"/>
       <c r="D416" s="1"/>
       <c r="E416" s="13"/>
     </row>
-    <row r="417" spans="2:5">
+    <row r="417" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B417" s="3"/>
       <c r="C417" s="1"/>
       <c r="D417" s="1"/>
       <c r="E417" s="13"/>
     </row>
-    <row r="418" spans="2:5">
+    <row r="418" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B418" s="3"/>
       <c r="C418" s="1"/>
       <c r="D418" s="1"/>
       <c r="E418" s="13"/>
     </row>
-    <row r="419" spans="2:5">
+    <row r="419" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B419" s="3"/>
       <c r="C419" s="1"/>
       <c r="D419" s="1"/>
       <c r="E419" s="13"/>
     </row>
-    <row r="420" spans="2:5">
+    <row r="420" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B420" s="3"/>
       <c r="C420" s="1"/>
       <c r="D420" s="1"/>
       <c r="E420" s="13"/>
     </row>
-    <row r="421" spans="2:5">
+    <row r="421" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B421" s="3"/>
       <c r="C421" s="1"/>
       <c r="D421" s="1"/>
       <c r="E421" s="13"/>
     </row>
-    <row r="422" spans="2:5">
+    <row r="422" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B422" s="3"/>
       <c r="C422" s="1"/>
       <c r="D422" s="1"/>
       <c r="E422" s="13"/>
     </row>
-    <row r="423" spans="2:5">
+    <row r="423" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B423" s="3"/>
       <c r="C423" s="1"/>
       <c r="D423" s="1"/>
       <c r="E423" s="13"/>
     </row>
-    <row r="424" spans="2:5">
+    <row r="424" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B424" s="3"/>
       <c r="C424" s="1"/>
       <c r="D424" s="1"/>
       <c r="E424" s="13"/>
     </row>
-    <row r="425" spans="2:5">
+    <row r="425" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B425" s="3"/>
       <c r="C425" s="1"/>
       <c r="D425" s="1"/>
       <c r="E425" s="13"/>
     </row>
-    <row r="426" spans="2:5">
+    <row r="426" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B426" s="3"/>
       <c r="C426" s="1"/>
       <c r="D426" s="1"/>
       <c r="E426" s="13"/>
     </row>
-    <row r="427" spans="2:5">
+    <row r="427" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B427" s="3"/>
       <c r="C427" s="1"/>
       <c r="D427" s="1"/>
       <c r="E427" s="13"/>
     </row>
-    <row r="428" spans="2:5">
+    <row r="428" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B428" s="3"/>
       <c r="C428" s="1"/>
       <c r="D428" s="1"/>
       <c r="E428" s="13"/>
     </row>
-    <row r="429" spans="2:5">
+    <row r="429" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B429" s="3"/>
       <c r="C429" s="1"/>
       <c r="D429" s="1"/>
       <c r="E429" s="13"/>
     </row>
-    <row r="430" spans="2:5">
+    <row r="430" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B430" s="3"/>
       <c r="C430" s="1"/>
       <c r="D430" s="1"/>
       <c r="E430" s="13"/>
     </row>
-    <row r="431" spans="2:5">
+    <row r="431" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B431" s="3"/>
       <c r="C431" s="1"/>
       <c r="D431" s="1"/>
       <c r="E431" s="13"/>
     </row>
-    <row r="432" spans="2:5">
+    <row r="432" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B432" s="3"/>
       <c r="C432" s="1"/>
       <c r="D432" s="1"/>
       <c r="E432" s="13"/>
     </row>
-    <row r="433" spans="2:5">
+    <row r="433" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B433" s="3"/>
       <c r="C433" s="1"/>
       <c r="D433" s="1"/>
       <c r="E433" s="13"/>
     </row>
-    <row r="434" spans="2:5">
+    <row r="434" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B434" s="3"/>
       <c r="C434" s="1"/>
       <c r="D434" s="1"/>
       <c r="E434" s="13"/>
     </row>
-    <row r="435" spans="2:5">
+    <row r="435" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B435" s="3"/>
       <c r="C435" s="1"/>
       <c r="D435" s="1"/>
       <c r="E435" s="13"/>
     </row>
-    <row r="436" spans="2:5">
+    <row r="436" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B436" s="3"/>
       <c r="C436" s="1"/>
       <c r="D436" s="1"/>
       <c r="E436" s="13"/>
     </row>
-    <row r="437" spans="2:5">
+    <row r="437" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B437" s="3"/>
       <c r="C437" s="1"/>
       <c r="D437" s="1"/>
       <c r="E437" s="13"/>
     </row>
-    <row r="438" spans="2:5">
+    <row r="438" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B438" s="3"/>
       <c r="C438" s="1"/>
       <c r="D438" s="1"/>
       <c r="E438" s="13"/>
     </row>
-    <row r="439" spans="2:5">
+    <row r="439" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B439" s="3"/>
       <c r="C439" s="1"/>
       <c r="D439" s="1"/>
       <c r="E439" s="13"/>
     </row>
-    <row r="440" spans="2:5">
+    <row r="440" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B440" s="3"/>
       <c r="C440" s="1"/>
       <c r="D440" s="1"/>
       <c r="E440" s="13"/>
     </row>
-    <row r="441" spans="2:5">
+    <row r="441" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B441" s="3"/>
       <c r="C441" s="1"/>
       <c r="D441" s="1"/>
       <c r="E441" s="13"/>
     </row>
-    <row r="442" spans="2:5">
+    <row r="442" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B442" s="3"/>
       <c r="C442" s="1"/>
       <c r="D442" s="1"/>
       <c r="E442" s="13"/>
     </row>
-    <row r="443" spans="2:5">
+    <row r="443" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B443" s="3"/>
       <c r="C443" s="1"/>
       <c r="D443" s="1"/>
       <c r="E443" s="13"/>
     </row>
-    <row r="444" spans="2:5">
+    <row r="444" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B444" s="3"/>
       <c r="C444" s="1"/>
       <c r="D444" s="1"/>
       <c r="E444" s="13"/>
     </row>
-    <row r="445" spans="2:5">
+    <row r="445" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B445" s="3"/>
       <c r="C445" s="1"/>
       <c r="D445" s="1"/>
       <c r="E445" s="13"/>
     </row>
-    <row r="446" spans="2:5">
+    <row r="446" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B446" s="3"/>
       <c r="C446" s="1"/>
       <c r="D446" s="1"/>
       <c r="E446" s="13"/>
     </row>
-    <row r="447" spans="2:5">
+    <row r="447" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B447" s="3"/>
       <c r="C447" s="1"/>
       <c r="D447" s="1"/>
       <c r="E447" s="13"/>
     </row>
-    <row r="448" spans="2:5">
+    <row r="448" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B448" s="3"/>
       <c r="C448" s="1"/>
       <c r="D448" s="1"/>
       <c r="E448" s="13"/>
     </row>
-    <row r="449" spans="2:5">
+    <row r="449" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B449" s="3"/>
       <c r="C449" s="1"/>
       <c r="D449" s="1"/>
       <c r="E449" s="13"/>
     </row>
-    <row r="450" spans="2:5">
+    <row r="450" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B450" s="3"/>
       <c r="C450" s="1"/>
       <c r="D450" s="1"/>
       <c r="E450" s="13"/>
     </row>
-    <row r="451" spans="2:5">
+    <row r="451" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B451" s="3"/>
       <c r="C451" s="1"/>
       <c r="D451" s="1"/>
       <c r="E451" s="13"/>
     </row>
-    <row r="452" spans="2:5">
+    <row r="452" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B452" s="3"/>
       <c r="C452" s="1"/>
       <c r="D452" s="1"/>
       <c r="E452" s="13"/>
     </row>
-    <row r="453" spans="2:5">
+    <row r="453" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B453" s="3"/>
       <c r="C453" s="1"/>
       <c r="D453" s="1"/>
       <c r="E453" s="13"/>
     </row>
-    <row r="454" spans="2:5">
+    <row r="454" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B454" s="3"/>
       <c r="C454" s="1"/>
       <c r="D454" s="1"/>
       <c r="E454" s="13"/>
     </row>
-    <row r="455" spans="2:5">
+    <row r="455" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B455" s="3"/>
       <c r="C455" s="1"/>
       <c r="D455" s="1"/>
       <c r="E455" s="13"/>
     </row>
-    <row r="456" spans="2:5">
+    <row r="456" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B456" s="3"/>
       <c r="C456" s="1"/>
       <c r="D456" s="1"/>
       <c r="E456" s="1"/>
     </row>
-    <row r="457" spans="2:5">
+    <row r="457" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B457" s="3"/>
       <c r="C457" s="1"/>
       <c r="D457" s="1"/>
       <c r="E457" s="1"/>
     </row>
-    <row r="458" spans="2:5">
+    <row r="458" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B458" s="3"/>
       <c r="C458" s="1"/>
       <c r="D458" s="1"/>
       <c r="E458" s="1"/>
     </row>
-    <row r="459" spans="2:5">
+    <row r="459" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B459" s="3"/>
       <c r="C459" s="1"/>
       <c r="D459" s="1"/>
       <c r="E459" s="1"/>
     </row>
-    <row r="460" spans="2:5">
+    <row r="460" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B460" s="3"/>
       <c r="C460" s="1"/>
       <c r="D460" s="1"/>
       <c r="E460" s="1"/>
     </row>
-    <row r="461" spans="2:5">
+    <row r="461" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B461" s="3"/>
       <c r="C461" s="1"/>
       <c r="D461" s="1"/>
       <c r="E461" s="1"/>
     </row>
-    <row r="462" spans="2:5">
+    <row r="462" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B462" s="3"/>
       <c r="C462" s="1"/>
       <c r="D462" s="1"/>
       <c r="E462" s="1"/>
     </row>
-    <row r="463" spans="2:5">
+    <row r="463" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B463" s="3"/>
       <c r="C463" s="1"/>
       <c r="D463" s="1"/>
       <c r="E463" s="1"/>
     </row>
-    <row r="464" spans="2:5">
+    <row r="464" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B464" s="3"/>
       <c r="C464" s="1"/>
       <c r="D464" s="1"/>
       <c r="E464" s="1"/>
     </row>
-    <row r="465" spans="2:2">
+    <row r="465" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B465" s="3"/>
     </row>
-    <row r="466" spans="2:2">
+    <row r="466" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B466" s="3"/>
     </row>
-    <row r="467" spans="2:2">
+    <row r="467" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B467" s="3"/>
     </row>
-    <row r="468" spans="2:2">
+    <row r="468" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B468" s="3"/>
     </row>
-    <row r="469" spans="2:2">
+    <row r="469" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B469" s="3"/>
     </row>
-    <row r="470" spans="2:2">
+    <row r="470" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B470" s="3"/>
     </row>
-    <row r="471" spans="2:2">
+    <row r="471" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B471" s="3"/>
     </row>
-    <row r="472" spans="2:2">
+    <row r="472" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B472" s="3"/>
     </row>
-    <row r="473" spans="2:2">
+    <row r="473" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B473" s="3"/>
     </row>
-    <row r="474" spans="2:2">
+    <row r="474" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B474" s="3"/>
     </row>
-    <row r="475" spans="2:2">
+    <row r="475" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B475" s="3"/>
     </row>
-    <row r="476" spans="2:2">
+    <row r="476" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B476" s="3"/>
     </row>
-    <row r="477" spans="2:2">
+    <row r="477" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B477" s="3"/>
     </row>
-    <row r="478" spans="2:2">
+    <row r="478" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B478" s="3"/>
     </row>
-    <row r="479" spans="2:2">
+    <row r="479" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B479" s="3"/>
     </row>
-    <row r="480" spans="2:2">
+    <row r="480" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B480" s="3"/>
     </row>
-    <row r="481" spans="2:2">
+    <row r="481" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B481" s="3"/>
     </row>
-    <row r="482" spans="2:2">
+    <row r="482" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B482" s="3"/>
     </row>
-    <row r="483" spans="2:2">
+    <row r="483" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B483" s="3"/>
     </row>
-    <row r="484" spans="2:2">
+    <row r="484" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B484" s="3"/>
     </row>
-    <row r="485" spans="2:2">
+    <row r="485" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B485" s="3"/>
     </row>
-    <row r="486" spans="2:2">
+    <row r="486" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B486" s="3"/>
     </row>
-    <row r="487" spans="2:2">
+    <row r="487" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B487" s="3"/>
     </row>
-    <row r="488" spans="2:2">
+    <row r="488" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B488" s="3"/>
     </row>
-    <row r="489" spans="2:2">
+    <row r="489" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B489" s="3"/>
     </row>
-    <row r="490" spans="2:2">
+    <row r="490" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B490" s="3"/>
     </row>
-    <row r="491" spans="2:2">
+    <row r="491" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B491" s="3"/>
     </row>
-    <row r="492" spans="2:2">
+    <row r="492" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B492" s="3"/>
     </row>
-    <row r="493" spans="2:2">
+    <row r="493" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B493" s="3"/>
     </row>
-    <row r="494" spans="2:2">
+    <row r="494" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B494" s="3"/>
     </row>
-    <row r="495" spans="2:2">
+    <row r="495" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B495" s="3"/>
     </row>
-    <row r="496" spans="2:2">
+    <row r="496" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B496" s="3"/>
     </row>
-    <row r="497" spans="2:2">
+    <row r="497" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B497" s="3"/>
     </row>
-    <row r="498" spans="2:2">
+    <row r="498" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B498" s="3"/>
     </row>
-    <row r="499" spans="2:2">
+    <row r="499" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B499" s="3"/>
     </row>
-    <row r="500" spans="2:2">
+    <row r="500" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B500" s="3"/>
     </row>
-    <row r="501" spans="2:2">
+    <row r="501" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B501" s="3"/>
     </row>
-    <row r="502" spans="2:2">
+    <row r="502" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B502" s="3"/>
     </row>
-    <row r="503" spans="2:2">
+    <row r="503" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B503" s="3"/>
     </row>
-    <row r="504" spans="2:2">
+    <row r="504" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B504" s="3"/>
     </row>
-    <row r="505" spans="2:2">
+    <row r="505" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B505" s="3"/>
     </row>
-    <row r="506" spans="2:2">
+    <row r="506" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B506" s="3"/>
     </row>
-    <row r="507" spans="2:2">
+    <row r="507" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B507" s="3"/>
     </row>
-    <row r="508" spans="2:2">
+    <row r="508" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B508" s="3"/>
     </row>
-    <row r="509" spans="2:2">
+    <row r="509" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B509" s="3"/>
     </row>
-    <row r="510" spans="2:2">
+    <row r="510" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B510" s="3"/>
     </row>
-    <row r="511" spans="2:2">
+    <row r="511" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B511" s="3"/>
     </row>
-    <row r="512" spans="2:2">
+    <row r="512" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B512" s="3"/>
     </row>
-    <row r="513" spans="2:2">
+    <row r="513" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B513" s="3"/>
     </row>
-    <row r="514" spans="2:2">
+    <row r="514" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B514" s="3"/>
     </row>
-    <row r="515" spans="2:2">
+    <row r="515" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B515" s="3"/>
     </row>
-    <row r="516" spans="2:2">
+    <row r="516" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B516" s="3"/>
     </row>
-    <row r="517" spans="2:2">
+    <row r="517" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B517" s="3"/>
     </row>
-    <row r="518" spans="2:2">
+    <row r="518" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B518" s="3"/>
     </row>
-    <row r="519" spans="2:2">
+    <row r="519" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B519" s="3"/>
     </row>
-    <row r="520" spans="2:2">
+    <row r="520" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B520" s="3"/>
     </row>
-    <row r="521" spans="2:2">
+    <row r="521" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B521" s="3"/>
     </row>
-    <row r="522" spans="2:2">
+    <row r="522" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B522" s="3"/>
     </row>
-    <row r="523" spans="2:2">
+    <row r="523" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B523" s="3"/>
     </row>
-    <row r="524" spans="2:2">
+    <row r="524" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B524" s="3"/>
     </row>
-    <row r="525" spans="2:2">
+    <row r="525" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B525" s="3"/>
     </row>
-    <row r="526" spans="2:2">
+    <row r="526" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B526" s="3"/>
     </row>
-    <row r="527" spans="2:2">
+    <row r="527" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B527" s="3"/>
     </row>
-    <row r="528" spans="2:2">
+    <row r="528" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B528" s="3"/>
     </row>
-    <row r="529" spans="2:2">
+    <row r="529" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B529" s="3"/>
     </row>
-    <row r="530" spans="2:2">
+    <row r="530" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B530" s="3"/>
     </row>
-    <row r="531" spans="2:2">
+    <row r="531" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B531" s="3"/>
     </row>
-    <row r="532" spans="2:2">
+    <row r="532" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B532" s="3"/>
     </row>
-    <row r="533" spans="2:2">
+    <row r="533" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B533" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="120" verticalDpi="72" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>